<commit_message>
presu acomodado para entrar bien. Recompilen y asegurense que se ve todo!!!
</commit_message>
<xml_diff>
--- a/Presupuesto/PRESUPUESTOS.xlsx
+++ b/Presupuesto/PRESUPUESTOS.xlsx
@@ -772,11 +772,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="183" formatCode="_ &quot;$&quot;\ * #,##0_ ;_ &quot;$&quot;\ * \-#,##0_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="_ &quot;$&quot;\ * #,##0_ ;_ &quot;$&quot;\ * \-#,##0_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1330,7 +1330,7 @@
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1339,9 +1339,9 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1364,7 +1364,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="8"/>
     <xf numFmtId="9" fontId="8" fillId="6" borderId="4" xfId="8" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="9" applyFont="1"/>
@@ -1377,9 +1377,9 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="9" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="7" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="17" borderId="5" xfId="9" applyFont="1" applyFill="1"/>
@@ -1391,31 +1391,31 @@
     <xf numFmtId="1" fontId="9" fillId="7" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="22" fillId="4" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="9" fillId="7" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="9" fillId="7" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="6" applyFont="1"/>
-    <xf numFmtId="169" fontId="23" fillId="5" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="23" fillId="5" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="6" applyFont="1"/>
-    <xf numFmtId="169" fontId="22" fillId="5" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="22" fillId="5" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="4" borderId="2" xfId="5" applyFont="1"/>
-    <xf numFmtId="169" fontId="23" fillId="4" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="23" fillId="4" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="5" applyFont="1"/>
-    <xf numFmtId="169" fontId="22" fillId="4" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="22" fillId="4" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="7" borderId="5" xfId="9" applyFont="1"/>
-    <xf numFmtId="169" fontId="23" fillId="7" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="23" fillId="7" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="9" applyFont="1"/>
-    <xf numFmtId="169" fontId="22" fillId="7" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="22" fillId="7" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="9" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="2" xfId="7" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="23" fillId="5" borderId="2" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="23" fillId="5" borderId="2" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="23" fillId="5" borderId="2" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="23" fillId="7" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="23" fillId="5" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="22" fillId="5" borderId="2" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="22" fillId="5" borderId="2" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="7" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1430,7 +1430,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1440,14 +1440,14 @@
     <xf numFmtId="0" fontId="22" fillId="22" borderId="2" xfId="5" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="183" fontId="9" fillId="11" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="22" fillId="22" borderId="2" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="26" fillId="9" borderId="10" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="9" fillId="11" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="22" fillId="22" borderId="2" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="26" fillId="9" borderId="10" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="23" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="26" fillId="0" borderId="12" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1455,39 +1455,39 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="21" fillId="12" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="21" fillId="12" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="9" borderId="3" xfId="6" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="23" fillId="5" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="23" fillId="5" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="7" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="23" fillId="5" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="23" fillId="5" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="6" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="22" fillId="5" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="22" fillId="5" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="16" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="16" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="23" fillId="16" borderId="6" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="23" fillId="16" borderId="6" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="6" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="7" borderId="6" xfId="9" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="23" fillId="7" borderId="6" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="23" fillId="7" borderId="6" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="7" borderId="6" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1508,22 +1508,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="9" fillId="0" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="19" borderId="6" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="9" fillId="19" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="9" fillId="19" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="23" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="22" fillId="23" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="22" fillId="23" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="20" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="15" borderId="2" xfId="5" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="23" fillId="15" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="23" fillId="15" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="23" fillId="15" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="15" borderId="2" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1551,26 +1551,11 @@
     <xf numFmtId="0" fontId="22" fillId="5" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1580,14 +1565,31 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="26" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="9" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="26" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="9" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Buena" xfId="3" builtinId="26"/>
@@ -2079,10 +2081,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R390"/>
+  <dimension ref="A1:R393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B318" sqref="B318"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A394" sqref="A1:P394"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2208,7 +2210,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" s="8" customFormat="1">
-      <c r="A16" s="174" t="s">
+      <c r="A16" s="169" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="8">
@@ -2247,7 +2249,7 @@
       <c r="M16" s="8">
         <v>1905</v>
       </c>
-      <c r="N16" s="174">
+      <c r="N16" s="169">
         <v>15160</v>
       </c>
     </row>
@@ -2460,37 +2462,37 @@
       </c>
     </row>
     <row r="60" spans="2:10">
-      <c r="B60" s="173" t="s">
+      <c r="B60" s="168" t="s">
         <v>50</v>
       </c>
-      <c r="C60" s="173"/>
-      <c r="D60" s="173" t="s">
+      <c r="C60" s="168"/>
+      <c r="D60" s="168" t="s">
         <v>45</v>
       </c>
-      <c r="E60" s="173"/>
-      <c r="F60" s="173"/>
-      <c r="G60" s="173" t="s">
+      <c r="E60" s="168"/>
+      <c r="F60" s="168"/>
+      <c r="G60" s="168" t="s">
         <v>49</v>
       </c>
       <c r="H60" s="85"/>
-      <c r="I60" s="173"/>
+      <c r="I60" s="168"/>
       <c r="J60" s="8"/>
     </row>
     <row r="61" spans="2:10">
-      <c r="B61" s="173" t="s">
+      <c r="B61" s="168" t="s">
         <v>51</v>
       </c>
-      <c r="C61" s="173"/>
-      <c r="D61" s="173"/>
-      <c r="E61" s="173"/>
-      <c r="F61" s="173"/>
-      <c r="G61" s="173"/>
+      <c r="C61" s="168"/>
+      <c r="D61" s="168"/>
+      <c r="E61" s="168"/>
+      <c r="F61" s="168"/>
+      <c r="G61" s="168"/>
       <c r="H61" s="85"/>
       <c r="I61" s="85"/>
       <c r="J61" s="8"/>
     </row>
     <row r="62" spans="2:10">
-      <c r="B62" s="173" t="s">
+      <c r="B62" s="168" t="s">
         <v>52</v>
       </c>
       <c r="C62" s="85"/>
@@ -2507,7 +2509,7 @@
       <c r="J62" s="8"/>
     </row>
     <row r="63" spans="2:10">
-      <c r="B63" s="173"/>
+      <c r="B63" s="168"/>
       <c r="C63" s="85"/>
       <c r="D63" s="85" t="s">
         <v>55</v>
@@ -2526,7 +2528,7 @@
       <c r="J63" s="8"/>
     </row>
     <row r="64" spans="2:10">
-      <c r="B64" s="173"/>
+      <c r="B64" s="168"/>
       <c r="C64" s="85"/>
       <c r="D64" s="85" t="s">
         <v>58</v>
@@ -2541,7 +2543,7 @@
       <c r="J64" s="8"/>
     </row>
     <row r="65" spans="1:10">
-      <c r="B65" s="173" t="s">
+      <c r="B65" s="168" t="s">
         <v>60</v>
       </c>
       <c r="C65" s="85"/>
@@ -2558,7 +2560,7 @@
       <c r="J65" s="8"/>
     </row>
     <row r="66" spans="1:10">
-      <c r="B66" s="173"/>
+      <c r="B66" s="168"/>
       <c r="C66" s="85"/>
       <c r="D66" s="85" t="s">
         <v>55</v>
@@ -2577,7 +2579,7 @@
       <c r="J66" s="8"/>
     </row>
     <row r="67" spans="1:10">
-      <c r="B67" s="173"/>
+      <c r="B67" s="168"/>
       <c r="C67" s="85"/>
       <c r="D67" s="85" t="s">
         <v>64</v>
@@ -2592,18 +2594,18 @@
       <c r="J67" s="8"/>
     </row>
     <row r="68" spans="1:10">
-      <c r="B68" s="173" t="s">
+      <c r="B68" s="168" t="s">
         <v>66</v>
       </c>
       <c r="C68" s="85"/>
       <c r="D68" s="85"/>
       <c r="E68" s="85"/>
-      <c r="F68" s="175" t="s">
+      <c r="F68" s="170" t="s">
         <v>67</v>
       </c>
-      <c r="G68" s="175"/>
-      <c r="H68" s="175"/>
-      <c r="I68" s="175"/>
+      <c r="G68" s="170"/>
+      <c r="H68" s="170"/>
+      <c r="I68" s="170"/>
       <c r="J68" s="8"/>
     </row>
     <row r="72" spans="1:10">
@@ -3948,7 +3950,7 @@
         <v>401.8</v>
       </c>
       <c r="C160" s="34">
-        <f t="shared" ref="B160:O160" si="6">C159*0.2</f>
+        <f t="shared" ref="C160:O160" si="6">C159*0.2</f>
         <v>394</v>
       </c>
       <c r="D160" s="34">
@@ -4013,7 +4015,7 @@
         <v>394</v>
       </c>
       <c r="C161" s="34">
-        <f t="shared" ref="C161:M161" si="7">D160</f>
+        <f t="shared" ref="C161:L161" si="7">D160</f>
         <v>421.40000000000003</v>
       </c>
       <c r="D161" s="34">
@@ -5488,55 +5490,55 @@
         <v>131</v>
       </c>
       <c r="B201" s="59">
-        <f>B168*$C180</f>
+        <f t="shared" ref="B201:N201" si="22">B168*$C180</f>
         <v>10976</v>
       </c>
       <c r="C201" s="59">
-        <f>C168*$C180</f>
+        <f t="shared" si="22"/>
         <v>12584</v>
       </c>
       <c r="D201" s="59">
-        <f>D168*$C180</f>
+        <f t="shared" si="22"/>
         <v>15016</v>
       </c>
       <c r="E201" s="59">
-        <f>E168*$C180</f>
+        <f t="shared" si="22"/>
         <v>11952</v>
       </c>
       <c r="F201" s="59">
-        <f>F168*$C180</f>
+        <f t="shared" si="22"/>
         <v>13588</v>
       </c>
       <c r="G201" s="59">
-        <f>G168*$C180</f>
+        <f t="shared" si="22"/>
         <v>13244</v>
       </c>
       <c r="H201" s="59">
-        <f>H168*$C180</f>
+        <f t="shared" si="22"/>
         <v>12740</v>
       </c>
       <c r="I201" s="59">
-        <f>I168*$C180</f>
+        <f t="shared" si="22"/>
         <v>20288</v>
       </c>
       <c r="J201" s="59">
-        <f>J168*$C180</f>
+        <f t="shared" si="22"/>
         <v>19316</v>
       </c>
       <c r="K201" s="59">
-        <f>K168*$C180</f>
+        <f t="shared" si="22"/>
         <v>18412</v>
       </c>
       <c r="L201" s="59">
-        <f>L168*$C180</f>
+        <f t="shared" si="22"/>
         <v>11884</v>
       </c>
       <c r="M201" s="59">
-        <f>M168*$C180</f>
+        <f t="shared" si="22"/>
         <v>12487.8</v>
       </c>
       <c r="N201" s="59">
-        <f>N168*$C180</f>
+        <f t="shared" si="22"/>
         <v>11432.19</v>
       </c>
       <c r="O201" s="59">
@@ -5552,51 +5554,51 @@
         <v>1097.6000000000001</v>
       </c>
       <c r="C202" s="59">
-        <f t="shared" ref="C202:N202" si="22">C201*0.1</f>
+        <f t="shared" ref="C202:N202" si="23">C201*0.1</f>
         <v>1258.4000000000001</v>
       </c>
       <c r="D202" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1501.6000000000001</v>
       </c>
       <c r="E202" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1195.2</v>
       </c>
       <c r="F202" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1358.8000000000002</v>
       </c>
       <c r="G202" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1324.4</v>
       </c>
       <c r="H202" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1274</v>
       </c>
       <c r="I202" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2028.8000000000002</v>
       </c>
       <c r="J202" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1931.6000000000001</v>
       </c>
       <c r="K202" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1841.2</v>
       </c>
       <c r="L202" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1188.4000000000001</v>
       </c>
       <c r="M202" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1248.78</v>
       </c>
       <c r="N202" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1143.2190000000001</v>
       </c>
       <c r="O202" s="59">
@@ -5612,43 +5614,43 @@
         <v>1258.4000000000001</v>
       </c>
       <c r="C203" s="59">
-        <f t="shared" ref="C203:L203" si="23">D202</f>
+        <f t="shared" ref="C203:L203" si="24">D202</f>
         <v>1501.6000000000001</v>
       </c>
       <c r="D203" s="59">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1195.2</v>
       </c>
       <c r="E203" s="59">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1358.8000000000002</v>
       </c>
       <c r="F203" s="59">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1324.4</v>
       </c>
       <c r="G203" s="59">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1274</v>
       </c>
       <c r="H203" s="59">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>2028.8000000000002</v>
       </c>
       <c r="I203" s="59">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1931.6000000000001</v>
       </c>
       <c r="J203" s="59">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1841.2</v>
       </c>
       <c r="K203" s="59">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1188.4000000000001</v>
       </c>
       <c r="L203" s="59">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1248.78</v>
       </c>
       <c r="M203" s="59">
@@ -5671,47 +5673,47 @@
         <v>11136.8</v>
       </c>
       <c r="C204" s="61">
-        <f t="shared" ref="C204:M204" si="24">(C203-C202)+C201</f>
+        <f t="shared" ref="C204:M204" si="25">(C203-C202)+C201</f>
         <v>12827.2</v>
       </c>
       <c r="D204" s="61">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>14709.6</v>
       </c>
       <c r="E204" s="61">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>12115.6</v>
       </c>
       <c r="F204" s="61">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>13553.6</v>
       </c>
       <c r="G204" s="61">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>13193.6</v>
       </c>
       <c r="H204" s="61">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>13494.8</v>
       </c>
       <c r="I204" s="61">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>20190.8</v>
       </c>
       <c r="J204" s="61">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>19225.599999999999</v>
       </c>
       <c r="K204" s="61">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>17759.2</v>
       </c>
       <c r="L204" s="61">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>11944.38</v>
       </c>
       <c r="M204" s="61">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>12382.239</v>
       </c>
       <c r="N204" s="61" t="s">
@@ -5881,47 +5883,47 @@
         <v>2001.2</v>
       </c>
       <c r="C214" s="65">
-        <f t="shared" ref="C214:M214" si="25">C162</f>
+        <f t="shared" ref="C214:M214" si="26">C162</f>
         <v>1997.4</v>
       </c>
       <c r="D214" s="65">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2131.6</v>
       </c>
       <c r="E214" s="65">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2234.4</v>
       </c>
       <c r="F214" s="65">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2194.6</v>
       </c>
       <c r="G214" s="65">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2097.4</v>
       </c>
       <c r="H214" s="65">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2619</v>
       </c>
       <c r="I214" s="65">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2605.8000000000002</v>
       </c>
       <c r="J214" s="65">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2595.1999999999998</v>
       </c>
       <c r="K214" s="65">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2257.4</v>
       </c>
       <c r="L214" s="65">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2204.1999999999998</v>
       </c>
       <c r="M214" s="65">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1945.89</v>
       </c>
     </row>
@@ -5934,47 +5936,47 @@
         <v>20.012</v>
       </c>
       <c r="C215" s="66">
-        <f t="shared" ref="C215:M215" si="26">C214/C212</f>
+        <f t="shared" ref="C215:M215" si="27">C214/C212</f>
         <v>19.974</v>
       </c>
       <c r="D215" s="66">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>21.315999999999999</v>
       </c>
       <c r="E215" s="66">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>22.344000000000001</v>
       </c>
       <c r="F215" s="66">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>21.945999999999998</v>
       </c>
       <c r="G215" s="66">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>20.974</v>
       </c>
       <c r="H215" s="66">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>26.19</v>
       </c>
       <c r="I215" s="66">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>26.058000000000003</v>
       </c>
       <c r="J215" s="66">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>25.951999999999998</v>
       </c>
       <c r="K215" s="66">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>22.574000000000002</v>
       </c>
       <c r="L215" s="66">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>22.041999999999998</v>
       </c>
       <c r="M215" s="66">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>19.4589</v>
       </c>
     </row>
@@ -5987,47 +5989,47 @@
         <v>0</v>
       </c>
       <c r="C216" s="66">
-        <f t="shared" ref="C216:M216" si="27">IF(C215 &gt; 24, C215 -24, 0)</f>
+        <f t="shared" ref="C216:M216" si="28">IF(C215 &gt; 24, C215 -24, 0)</f>
         <v>0</v>
       </c>
       <c r="D216" s="66">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="E216" s="66">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="F216" s="66">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="G216" s="66">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H216" s="69">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>2.1900000000000013</v>
       </c>
       <c r="I216" s="69">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>2.0580000000000034</v>
       </c>
       <c r="J216" s="69">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>1.9519999999999982</v>
       </c>
       <c r="K216" s="66">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="L216" s="66">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="M216" s="66">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -6040,47 +6042,47 @@
         <v>3.9879999999999995</v>
       </c>
       <c r="C217" s="66">
-        <f t="shared" ref="C217:M217" si="28">IF(C215 &lt; 24, 24 -C215,0)</f>
+        <f t="shared" ref="C217:M217" si="29">IF(C215 &lt; 24, 24 -C215,0)</f>
         <v>4.0259999999999998</v>
       </c>
       <c r="D217" s="66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>2.6840000000000011</v>
       </c>
       <c r="E217" s="66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.6559999999999988</v>
       </c>
       <c r="F217" s="66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>2.054000000000002</v>
       </c>
       <c r="G217" s="66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3.0259999999999998</v>
       </c>
       <c r="H217" s="66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="I217" s="66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="J217" s="66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="K217" s="66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.4259999999999984</v>
       </c>
       <c r="L217" s="66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.958000000000002</v>
       </c>
       <c r="M217" s="66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>4.5411000000000001</v>
       </c>
     </row>
@@ -6227,47 +6229,47 @@
         <v>2001.2</v>
       </c>
       <c r="C223" s="67">
-        <f t="shared" ref="C223:M223" si="29">C162</f>
+        <f t="shared" ref="C223:M223" si="30">C162</f>
         <v>1997.4</v>
       </c>
       <c r="D223" s="67">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>2131.6</v>
       </c>
       <c r="E223" s="67">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>2234.4</v>
       </c>
       <c r="F223" s="67">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>2194.6</v>
       </c>
       <c r="G223" s="67">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>2097.4</v>
       </c>
       <c r="H223" s="67">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>2619</v>
       </c>
       <c r="I223" s="67">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>2605.8000000000002</v>
       </c>
       <c r="J223" s="67">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>2595.1999999999998</v>
       </c>
       <c r="K223" s="67">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>2257.4</v>
       </c>
       <c r="L223" s="67">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>2204.1999999999998</v>
       </c>
       <c r="M223" s="67">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1945.89</v>
       </c>
     </row>
@@ -6280,47 +6282,47 @@
         <v>25.015000000000001</v>
       </c>
       <c r="C224" s="58">
-        <f t="shared" ref="C224:M224" si="30">C223/C221</f>
+        <f t="shared" ref="C224:M224" si="31">C223/C221</f>
         <v>24.967500000000001</v>
       </c>
       <c r="D224" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>26.645</v>
       </c>
       <c r="E224" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>27.93</v>
       </c>
       <c r="F224" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>27.432499999999997</v>
       </c>
       <c r="G224" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>26.217500000000001</v>
       </c>
       <c r="H224" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>32.737499999999997</v>
       </c>
       <c r="I224" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>32.572500000000005</v>
       </c>
       <c r="J224" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>32.44</v>
       </c>
       <c r="K224" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>28.217500000000001</v>
       </c>
       <c r="L224" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>27.552499999999998</v>
       </c>
       <c r="M224" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>24.323625</v>
       </c>
     </row>
@@ -6333,47 +6335,47 @@
         <v>1.0150000000000006</v>
       </c>
       <c r="C225" s="58">
-        <f t="shared" ref="C225:M225" si="31">IF(C224 &gt; 24, C224 -24, 0)</f>
+        <f t="shared" ref="C225:M225" si="32">IF(C224 &gt; 24, C224 -24, 0)</f>
         <v>0.96750000000000114</v>
       </c>
       <c r="D225" s="58">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>2.6449999999999996</v>
       </c>
       <c r="E225" s="58">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>3.9299999999999997</v>
       </c>
       <c r="F225" s="58">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>3.4324999999999974</v>
       </c>
       <c r="G225" s="58">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>2.2175000000000011</v>
       </c>
       <c r="H225" s="58">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>8.7374999999999972</v>
       </c>
       <c r="I225" s="58">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>8.5725000000000051</v>
       </c>
       <c r="J225" s="58">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>8.4399999999999977</v>
       </c>
       <c r="K225" s="58">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>4.2175000000000011</v>
       </c>
       <c r="L225" s="58">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>3.5524999999999984</v>
       </c>
       <c r="M225" s="58">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.32362499999999983</v>
       </c>
     </row>
@@ -6386,47 +6388,47 @@
         <v>0</v>
       </c>
       <c r="C226" s="58">
-        <f t="shared" ref="C226:M226" si="32">IF(C224 &lt; 24, 24 -C224,0)</f>
+        <f t="shared" ref="C226:M226" si="33">IF(C224 &lt; 24, 24 -C224,0)</f>
         <v>0</v>
       </c>
       <c r="D226" s="58">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="E226" s="58">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="F226" s="58">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="G226" s="58">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="H226" s="58">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="I226" s="58">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="J226" s="58">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="K226" s="58">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="L226" s="58">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="M226" s="58">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -6578,47 +6580,47 @@
         <v>548.79999999999995</v>
       </c>
       <c r="C233" s="146">
-        <f t="shared" ref="C233:M233" si="33">C168</f>
+        <f t="shared" ref="C233:M233" si="34">C168</f>
         <v>629.20000000000005</v>
       </c>
       <c r="D233" s="146">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>750.8</v>
       </c>
       <c r="E233" s="146">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>597.6</v>
       </c>
       <c r="F233" s="146">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>679.4</v>
       </c>
       <c r="G233" s="146">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>662.2</v>
       </c>
       <c r="H233" s="146">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>637</v>
       </c>
       <c r="I233" s="146">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1014.4</v>
       </c>
       <c r="J233" s="146">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>965.8</v>
       </c>
       <c r="K233" s="146">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>920.6</v>
       </c>
       <c r="L233" s="146">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>594.20000000000005</v>
       </c>
       <c r="M233" s="146">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>624.39</v>
       </c>
     </row>
@@ -6631,47 +6633,47 @@
         <v>4.9890909090909084</v>
       </c>
       <c r="C234" s="146">
-        <f t="shared" ref="C234:M234" si="34">C233/C231</f>
+        <f t="shared" ref="C234:M234" si="35">C233/C231</f>
         <v>5.7200000000000006</v>
       </c>
       <c r="D234" s="146">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>6.8254545454545452</v>
       </c>
       <c r="E234" s="146">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>5.4327272727272726</v>
       </c>
       <c r="F234" s="146">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>6.1763636363636358</v>
       </c>
       <c r="G234" s="146">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>6.0200000000000005</v>
       </c>
       <c r="H234" s="146">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>5.790909090909091</v>
       </c>
       <c r="I234" s="146">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>9.2218181818181808</v>
       </c>
       <c r="J234" s="146">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>8.7799999999999994</v>
       </c>
       <c r="K234" s="146">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>8.3690909090909091</v>
       </c>
       <c r="L234" s="146">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>5.4018181818181823</v>
       </c>
       <c r="M234" s="146">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>5.6762727272727274</v>
       </c>
     </row>
@@ -6684,47 +6686,47 @@
         <v>0</v>
       </c>
       <c r="C235" s="146">
-        <f t="shared" ref="C235:M235" si="35">IF(C234 &gt; 24, C234 -24, 0)</f>
+        <f t="shared" ref="C235:M235" si="36">IF(C234 &gt; 24, C234 -24, 0)</f>
         <v>0</v>
       </c>
       <c r="D235" s="146">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="E235" s="146">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="F235" s="146">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="G235" s="146">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="H235" s="146">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="I235" s="146">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="J235" s="146">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="K235" s="146">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="L235" s="146">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="M235" s="146">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -6737,47 +6739,47 @@
         <v>19.010909090909092</v>
       </c>
       <c r="C236" s="147">
-        <f t="shared" ref="C236:M236" si="36">IF(C234 &lt; 24, 24 -C234,0)</f>
+        <f t="shared" ref="C236:M236" si="37">IF(C234 &lt; 24, 24 -C234,0)</f>
         <v>18.28</v>
       </c>
       <c r="D236" s="147">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>17.174545454545456</v>
       </c>
       <c r="E236" s="147">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>18.567272727272726</v>
       </c>
       <c r="F236" s="147">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>17.823636363636364</v>
       </c>
       <c r="G236" s="147">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>17.98</v>
       </c>
       <c r="H236" s="147">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>18.209090909090911</v>
       </c>
       <c r="I236" s="147">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>14.778181818181819</v>
       </c>
       <c r="J236" s="147">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>15.22</v>
       </c>
       <c r="K236" s="147">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>15.630909090909091</v>
       </c>
       <c r="L236" s="147">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>18.598181818181818</v>
       </c>
       <c r="M236" s="147">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>18.323727272727272</v>
       </c>
     </row>
@@ -6924,47 +6926,47 @@
         <v>548.79999999999995</v>
       </c>
       <c r="C242" s="68">
-        <f t="shared" ref="C242:M242" si="37">C168</f>
+        <f t="shared" ref="C242:M242" si="38">C168</f>
         <v>629.20000000000005</v>
       </c>
       <c r="D242" s="68">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>750.8</v>
       </c>
       <c r="E242" s="68">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>597.6</v>
       </c>
       <c r="F242" s="68">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>679.4</v>
       </c>
       <c r="G242" s="68">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>662.2</v>
       </c>
       <c r="H242" s="68">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>637</v>
       </c>
       <c r="I242" s="68">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>1014.4</v>
       </c>
       <c r="J242" s="68">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>965.8</v>
       </c>
       <c r="K242" s="68">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>920.6</v>
       </c>
       <c r="L242" s="68">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>594.20000000000005</v>
       </c>
       <c r="M242" s="68">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>624.39</v>
       </c>
     </row>
@@ -6977,47 +6979,47 @@
         <v>6.0977777777777771</v>
       </c>
       <c r="C243" s="48">
-        <f t="shared" ref="C243:M243" si="38">C242/C240</f>
+        <f t="shared" ref="C243:M243" si="39">C242/C240</f>
         <v>6.9911111111111115</v>
       </c>
       <c r="D243" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>8.3422222222222224</v>
       </c>
       <c r="E243" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6.6400000000000006</v>
       </c>
       <c r="F243" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>7.5488888888888885</v>
       </c>
       <c r="G243" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>7.3577777777777786</v>
       </c>
       <c r="H243" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>7.0777777777777775</v>
       </c>
       <c r="I243" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>11.271111111111111</v>
       </c>
       <c r="J243" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>10.73111111111111</v>
       </c>
       <c r="K243" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>10.228888888888889</v>
       </c>
       <c r="L243" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6.6022222222222231</v>
       </c>
       <c r="M243" s="48">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6.9376666666666669</v>
       </c>
     </row>
@@ -7030,47 +7032,47 @@
         <v>0</v>
       </c>
       <c r="C244" s="48">
-        <f t="shared" ref="C244:M244" si="39">IF(C243 &gt; 24, C243 -24, 0)</f>
+        <f t="shared" ref="C244:M244" si="40">IF(C243 &gt; 24, C243 -24, 0)</f>
         <v>0</v>
       </c>
       <c r="D244" s="48">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="E244" s="48">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="F244" s="48">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="G244" s="48">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="H244" s="48">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="I244" s="48">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="J244" s="48">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K244" s="48">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="L244" s="48">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="M244" s="48">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
@@ -7083,47 +7085,47 @@
         <v>17.902222222222221</v>
       </c>
       <c r="C245" s="48">
-        <f t="shared" ref="C245:M245" si="40">IF(C243 &lt; 24, 24 -C243,0)</f>
+        <f t="shared" ref="C245:M245" si="41">IF(C243 &lt; 24, 24 -C243,0)</f>
         <v>17.00888888888889</v>
       </c>
       <c r="D245" s="48">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>15.657777777777778</v>
       </c>
       <c r="E245" s="48">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>17.36</v>
       </c>
       <c r="F245" s="48">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>16.451111111111111</v>
       </c>
       <c r="G245" s="48">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>16.642222222222223</v>
       </c>
       <c r="H245" s="48">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>16.922222222222224</v>
       </c>
       <c r="I245" s="48">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>12.728888888888889</v>
       </c>
       <c r="J245" s="48">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>13.26888888888889</v>
       </c>
       <c r="K245" s="48">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>13.771111111111111</v>
       </c>
       <c r="L245" s="48">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>17.397777777777776</v>
       </c>
       <c r="M245" s="48">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>17.062333333333335</v>
       </c>
     </row>
@@ -7132,51 +7134,51 @@
         <v>223</v>
       </c>
       <c r="B247" s="80">
-        <f>B243+B234+B225+B216</f>
+        <f t="shared" ref="B247:M247" si="42">B243+B234+B225+B216</f>
         <v>12.101868686868686</v>
       </c>
       <c r="C247" s="80">
-        <f>C243+C234+C225+C216</f>
+        <f t="shared" si="42"/>
         <v>13.678611111111113</v>
       </c>
       <c r="D247" s="80">
-        <f>D243+D234+D225+D216</f>
+        <f t="shared" si="42"/>
         <v>17.812676767676766</v>
       </c>
       <c r="E247" s="80">
-        <f>E243+E234+E225+E216</f>
+        <f t="shared" si="42"/>
         <v>16.002727272727274</v>
       </c>
       <c r="F247" s="80">
-        <f>F243+F234+F225+F216</f>
+        <f t="shared" si="42"/>
         <v>17.157752525252523</v>
       </c>
       <c r="G247" s="80">
-        <f>G243+G234+G225+G216</f>
+        <f t="shared" si="42"/>
         <v>15.595277777777781</v>
       </c>
       <c r="H247" s="80">
-        <f>H243+H234+H225+H216</f>
+        <f t="shared" si="42"/>
         <v>23.796186868686867</v>
       </c>
       <c r="I247" s="80">
-        <f>I243+I234+I225+I216</f>
+        <f t="shared" si="42"/>
         <v>31.123429292929298</v>
       </c>
       <c r="J247" s="80">
-        <f>J243+J234+J225+J216</f>
+        <f t="shared" si="42"/>
         <v>29.903111111111105</v>
       </c>
       <c r="K247" s="80">
-        <f>K243+K234+K225+K216</f>
+        <f t="shared" si="42"/>
         <v>22.815479797979798</v>
       </c>
       <c r="L247" s="80">
-        <f>L243+L234+L225+L216</f>
+        <f t="shared" si="42"/>
         <v>15.556540404040405</v>
       </c>
       <c r="M247" s="115">
-        <f>M243+M234+M225+M216</f>
+        <f t="shared" si="42"/>
         <v>12.937564393939393</v>
       </c>
       <c r="N247" s="116"/>
@@ -7194,47 +7196,47 @@
         <v>11.898131313131314</v>
       </c>
       <c r="C248" s="80">
-        <f t="shared" ref="C248:M248" si="41">24-C247</f>
+        <f t="shared" ref="C248:M248" si="43">24-C247</f>
         <v>10.321388888888887</v>
       </c>
       <c r="D248" s="80">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>6.1873232323232337</v>
       </c>
       <c r="E248" s="80">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>7.9972727272727262</v>
       </c>
       <c r="F248" s="80">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>6.8422474747474773</v>
       </c>
       <c r="G248" s="80">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>8.4047222222222189</v>
       </c>
       <c r="H248" s="80">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>0.20381313131313306</v>
       </c>
       <c r="I248" s="144">
-        <f t="shared" ref="I248" si="42">24-I247</f>
+        <f t="shared" ref="I248" si="44">24-I247</f>
         <v>-7.1234292929292984</v>
       </c>
       <c r="J248" s="144">
-        <f t="shared" ref="J248" si="43">24-J247</f>
+        <f t="shared" ref="J248" si="45">24-J247</f>
         <v>-5.9031111111111052</v>
       </c>
       <c r="K248" s="80">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>1.1845202020202024</v>
       </c>
       <c r="L248" s="80">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>8.4434595959595953</v>
       </c>
       <c r="M248" s="115">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>11.062435606060607</v>
       </c>
       <c r="N248" s="116"/>
@@ -7244,12 +7246,12 @@
       <c r="R248" s="116"/>
     </row>
     <row r="250" spans="1:18">
-      <c r="A250" s="164" t="s">
+      <c r="A250" s="159" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="251" spans="1:18">
-      <c r="A251" s="165" t="s">
+      <c r="A251" s="160" t="s">
         <v>181</v>
       </c>
       <c r="B251" t="s">
@@ -7257,7 +7259,7 @@
       </c>
     </row>
     <row r="252" spans="1:18">
-      <c r="A252" s="165" t="s">
+      <c r="A252" s="160" t="s">
         <v>181</v>
       </c>
       <c r="B252" t="s">
@@ -7265,7 +7267,7 @@
       </c>
     </row>
     <row r="253" spans="1:18">
-      <c r="A253" s="165" t="s">
+      <c r="A253" s="160" t="s">
         <v>181</v>
       </c>
       <c r="B253" t="s">
@@ -7273,7 +7275,7 @@
       </c>
     </row>
     <row r="254" spans="1:18">
-      <c r="A254" s="165" t="s">
+      <c r="A254" s="160" t="s">
         <v>181</v>
       </c>
       <c r="B254" t="s">
@@ -7281,48 +7283,48 @@
       </c>
     </row>
     <row r="255" spans="1:18">
-      <c r="A255" s="165" t="s">
+      <c r="A255" s="160" t="s">
         <v>181</v>
       </c>
-      <c r="B255" s="166" t="s">
+      <c r="B255" s="161" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="256" spans="1:18">
-      <c r="A256" s="165" t="s">
+      <c r="A256" s="160" t="s">
         <v>181</v>
       </c>
-      <c r="B256" s="166" t="s">
+      <c r="B256" s="161" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="257" spans="1:14">
-      <c r="A257" s="165" t="s">
+      <c r="A257" s="160" t="s">
         <v>181</v>
       </c>
-      <c r="B257" s="166" t="s">
+      <c r="B257" s="161" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="258" spans="1:14">
-      <c r="A258" s="165" t="s">
+      <c r="A258" s="160" t="s">
         <v>181</v>
       </c>
-      <c r="B258" s="166" t="s">
+      <c r="B258" s="161" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="259" spans="1:14">
-      <c r="A259" s="165" t="s">
+      <c r="A259" s="160" t="s">
         <v>181</v>
       </c>
-      <c r="B259" s="166" t="s">
+      <c r="B259" s="161" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="260" spans="1:14">
-      <c r="A260" s="165"/>
-      <c r="B260" s="165" t="s">
+      <c r="A260" s="160"/>
+      <c r="B260" s="160" t="s">
         <v>181</v>
       </c>
       <c r="C260" t="s">
@@ -7330,8 +7332,8 @@
       </c>
     </row>
     <row r="261" spans="1:14">
-      <c r="A261" s="165"/>
-      <c r="B261" s="165" t="s">
+      <c r="A261" s="160"/>
+      <c r="B261" s="160" t="s">
         <v>181</v>
       </c>
       <c r="C261" t="s">
@@ -7339,8 +7341,8 @@
       </c>
     </row>
     <row r="262" spans="1:14">
-      <c r="A262" s="165"/>
-      <c r="B262" s="165" t="s">
+      <c r="A262" s="160"/>
+      <c r="B262" s="160" t="s">
         <v>181</v>
       </c>
       <c r="C262" t="s">
@@ -7348,18 +7350,18 @@
       </c>
     </row>
     <row r="263" spans="1:14">
-      <c r="A263" s="165" t="s">
+      <c r="A263" s="160" t="s">
         <v>181</v>
       </c>
-      <c r="B263" s="166" t="s">
+      <c r="B263" s="161" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="264" spans="1:14">
-      <c r="A264" s="165" t="s">
+      <c r="A264" s="160" t="s">
         <v>181</v>
       </c>
-      <c r="B264" s="166" t="s">
+      <c r="B264" s="161" t="s">
         <v>248</v>
       </c>
     </row>
@@ -7435,47 +7437,47 @@
         <v>26112</v>
       </c>
       <c r="C270" s="82">
-        <f t="shared" ref="C270:M270" si="44">(C215+C217) *$C$210</f>
+        <f t="shared" ref="C270:M270" si="46">(C215+C217) *$C$210</f>
         <v>26112</v>
       </c>
       <c r="D270" s="82">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>26112</v>
       </c>
       <c r="E270" s="82">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>26112</v>
       </c>
       <c r="F270" s="82">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>26112</v>
       </c>
       <c r="G270" s="82">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>26112</v>
       </c>
       <c r="H270" s="82">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>28494.720000000001</v>
       </c>
       <c r="I270" s="82">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>28351.104000000003</v>
       </c>
       <c r="J270" s="82">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>28235.775999999998</v>
       </c>
       <c r="K270" s="82">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>26112</v>
       </c>
       <c r="L270" s="82">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>26112</v>
       </c>
       <c r="M270" s="82">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>26112</v>
       </c>
       <c r="N270" s="82">
@@ -7492,27 +7494,27 @@
         <v>23322.880000000001</v>
       </c>
       <c r="C271" s="82">
-        <f t="shared" ref="C271:M271" si="45">(C224+C225) *$C$219</f>
+        <f t="shared" ref="C271:M271" si="47">(C224+C225) *$C$219</f>
         <v>23237.760000000002</v>
       </c>
       <c r="D271" s="82">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>26243.84</v>
       </c>
       <c r="E271" s="82">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>28546.559999999998</v>
       </c>
       <c r="F271" s="82">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>27655.039999999994</v>
       </c>
       <c r="G271" s="82">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>25477.760000000002</v>
       </c>
       <c r="H271" s="82">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>37161.599999999991</v>
       </c>
       <c r="I271" s="83">
@@ -7524,19 +7526,19 @@
         <v>44562.261333333321</v>
       </c>
       <c r="K271" s="82">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>29061.760000000002</v>
       </c>
       <c r="L271" s="82">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>27870.079999999998</v>
       </c>
       <c r="M271" s="82">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>22083.936000000002</v>
       </c>
       <c r="N271" s="82">
-        <f t="shared" ref="N271:N277" si="46">SUM(B271:M271)</f>
+        <f t="shared" ref="N271:N277" si="48">SUM(B271:M271)</f>
         <v>361663.28630303033</v>
       </c>
     </row>
@@ -7549,51 +7551,51 @@
         <v>5029.0036363636355</v>
       </c>
       <c r="C272" s="82">
-        <f t="shared" ref="C272:M272" si="47">C234*$C$229</f>
+        <f t="shared" ref="C272:M272" si="49">C234*$C$229</f>
         <v>5765.76</v>
       </c>
       <c r="D272" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>6880.0581818181818</v>
       </c>
       <c r="E272" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>5476.1890909090907</v>
       </c>
       <c r="F272" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>6225.7745454545448</v>
       </c>
       <c r="G272" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>6068.1600000000008</v>
       </c>
       <c r="H272" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>5837.2363636363634</v>
       </c>
       <c r="I272" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>9295.5927272727258</v>
       </c>
       <c r="J272" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>8850.24</v>
       </c>
       <c r="K272" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>8436.0436363636363</v>
       </c>
       <c r="L272" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>5445.0327272727282</v>
       </c>
       <c r="M272" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>5721.6829090909096</v>
       </c>
       <c r="N272" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>79030.773818181828</v>
       </c>
     </row>
@@ -7606,51 +7608,51 @@
         <v>7561.2444444444436</v>
       </c>
       <c r="C273" s="82">
-        <f t="shared" ref="C273:M273" si="48">C243*$C$238</f>
+        <f t="shared" ref="C273:M273" si="50">C243*$C$238</f>
         <v>8668.9777777777781</v>
       </c>
       <c r="D273" s="82">
+        <f t="shared" si="50"/>
+        <v>10344.355555555556</v>
+      </c>
+      <c r="E273" s="82">
+        <f t="shared" si="50"/>
+        <v>8233.6</v>
+      </c>
+      <c r="F273" s="82">
+        <f t="shared" si="50"/>
+        <v>9360.6222222222223</v>
+      </c>
+      <c r="G273" s="82">
+        <f t="shared" si="50"/>
+        <v>9123.644444444446</v>
+      </c>
+      <c r="H273" s="82">
+        <f t="shared" si="50"/>
+        <v>8776.4444444444434</v>
+      </c>
+      <c r="I273" s="82">
+        <f t="shared" si="50"/>
+        <v>13976.177777777777</v>
+      </c>
+      <c r="J273" s="82">
+        <f t="shared" si="50"/>
+        <v>13306.577777777777</v>
+      </c>
+      <c r="K273" s="82">
+        <f t="shared" si="50"/>
+        <v>12683.822222222223</v>
+      </c>
+      <c r="L273" s="82">
+        <f t="shared" si="50"/>
+        <v>8186.7555555555564</v>
+      </c>
+      <c r="M273" s="82">
+        <f t="shared" si="50"/>
+        <v>8602.7066666666669</v>
+      </c>
+      <c r="N273" s="82">
         <f t="shared" si="48"/>
-        <v>10344.355555555556</v>
-      </c>
-      <c r="E273" s="82">
-        <f t="shared" si="48"/>
-        <v>8233.6</v>
-      </c>
-      <c r="F273" s="82">
-        <f t="shared" si="48"/>
-        <v>9360.6222222222223</v>
-      </c>
-      <c r="G273" s="82">
-        <f t="shared" si="48"/>
-        <v>9123.644444444446</v>
-      </c>
-      <c r="H273" s="82">
-        <f t="shared" si="48"/>
-        <v>8776.4444444444434</v>
-      </c>
-      <c r="I273" s="82">
-        <f t="shared" si="48"/>
-        <v>13976.177777777777</v>
-      </c>
-      <c r="J273" s="82">
-        <f t="shared" si="48"/>
-        <v>13306.577777777777</v>
-      </c>
-      <c r="K273" s="82">
-        <f t="shared" si="48"/>
-        <v>12683.822222222223</v>
-      </c>
-      <c r="L273" s="82">
-        <f t="shared" si="48"/>
-        <v>8186.7555555555564</v>
-      </c>
-      <c r="M273" s="82">
-        <f t="shared" si="48"/>
-        <v>8602.7066666666669</v>
-      </c>
-      <c r="N273" s="82">
-        <f t="shared" si="46"/>
         <v>118824.9288888889</v>
       </c>
     </row>
@@ -7663,27 +7665,27 @@
         <v>10660.725656565657</v>
       </c>
       <c r="C274" s="82">
-        <f t="shared" ref="C274:M274" si="49">C248*$C$219</f>
+        <f t="shared" ref="C274:M274" si="51">C248*$C$219</f>
         <v>9247.9644444444421</v>
       </c>
       <c r="D274" s="82">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>5543.8416161616169</v>
       </c>
       <c r="E274" s="82">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>7165.5563636363622</v>
       </c>
       <c r="F274" s="82">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>6130.6537373737392</v>
       </c>
       <c r="G274" s="82">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>7530.6311111111081</v>
       </c>
       <c r="H274" s="82">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>182.61656565656722</v>
       </c>
       <c r="I274" s="82">
@@ -7693,19 +7695,19 @@
         <v>0</v>
       </c>
       <c r="K274" s="82">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>1061.3301010101013</v>
       </c>
       <c r="L274" s="82">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>7565.3397979797974</v>
       </c>
       <c r="M274" s="82">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>9911.9423030303042</v>
       </c>
       <c r="N274" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>65000.601696969694</v>
       </c>
     </row>
@@ -7718,51 +7720,51 @@
         <v>72685.853737373734</v>
       </c>
       <c r="C275" s="84">
-        <f t="shared" ref="C275:M275" si="50">SUM(C270:C274)</f>
+        <f t="shared" ref="C275:M275" si="52">SUM(C270:C274)</f>
         <v>73032.462222222224</v>
       </c>
       <c r="D275" s="84">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>75124.095353535347</v>
       </c>
       <c r="E275" s="84">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>75533.905454545456</v>
       </c>
       <c r="F275" s="84">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>75484.090505050495</v>
       </c>
       <c r="G275" s="84">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>74312.195555555561</v>
       </c>
       <c r="H275" s="84">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>80452.617373737361</v>
       </c>
       <c r="I275" s="84">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>98062.683474747493</v>
       </c>
       <c r="J275" s="84">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>94954.855111111101</v>
       </c>
       <c r="K275" s="84">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>77354.955959595958</v>
       </c>
       <c r="L275" s="84">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>75179.208080808094</v>
       </c>
       <c r="M275" s="84">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>72432.267878787883</v>
       </c>
       <c r="N275" s="84">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>944609.19070707052</v>
       </c>
     </row>
@@ -7775,51 +7777,51 @@
         <v>58148.682989898989</v>
       </c>
       <c r="C276" s="82">
-        <f t="shared" ref="C276:M276" si="51">C275*0.8</f>
+        <f t="shared" ref="C276:M276" si="53">C275*0.8</f>
         <v>58425.969777777784</v>
       </c>
       <c r="D276" s="82">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>60099.276282828279</v>
       </c>
       <c r="E276" s="82">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>60427.124363636365</v>
       </c>
       <c r="F276" s="82">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>60387.272404040399</v>
       </c>
       <c r="G276" s="82">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>59449.756444444451</v>
       </c>
       <c r="H276" s="82">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>64362.093898989893</v>
       </c>
       <c r="I276" s="82">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>78450.146779798</v>
       </c>
       <c r="J276" s="82">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>75963.884088888881</v>
       </c>
       <c r="K276" s="82">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>61883.964767676771</v>
       </c>
       <c r="L276" s="82">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>60143.366464646475</v>
       </c>
       <c r="M276" s="82">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>57945.814303030311</v>
       </c>
       <c r="N276" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>755687.35256565665</v>
       </c>
     </row>
@@ -7832,51 +7834,51 @@
         <v>130834.53672727273</v>
       </c>
       <c r="C277" s="90">
-        <f t="shared" ref="C277:M277" si="52">SUM(C275:C276)</f>
+        <f t="shared" ref="C277:M277" si="54">SUM(C275:C276)</f>
         <v>131458.432</v>
       </c>
       <c r="D277" s="90">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>135223.37163636362</v>
       </c>
       <c r="E277" s="90">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>135961.02981818182</v>
       </c>
       <c r="F277" s="90">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>135871.36290909088</v>
       </c>
       <c r="G277" s="90">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>133761.95200000002</v>
       </c>
       <c r="H277" s="90">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>144814.71127272726</v>
       </c>
       <c r="I277" s="90">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>176512.83025454549</v>
       </c>
       <c r="J277" s="90">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>170918.73919999998</v>
       </c>
       <c r="K277" s="90">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>139238.92072727272</v>
       </c>
       <c r="L277" s="90">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>135322.57454545458</v>
       </c>
       <c r="M277" s="90">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>130378.0821818182</v>
       </c>
       <c r="N277" s="90">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1700296.5432727272</v>
       </c>
     </row>
@@ -8233,31 +8235,31 @@
         <v>705826.39999999991</v>
       </c>
       <c r="G295" s="91">
-        <f t="shared" ref="G295:M295" si="53">G291+G292+G293+G294</f>
+        <f t="shared" ref="G295:M295" si="55">G291+G292+G293+G294</f>
         <v>692302.8</v>
       </c>
       <c r="H295" s="91">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>804488.4</v>
       </c>
       <c r="I295" s="91">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>901952.2</v>
       </c>
       <c r="J295" s="91">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>877510.59999999986</v>
       </c>
       <c r="K295" s="91">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>784366.4</v>
       </c>
       <c r="L295" s="91">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>680190.57000000007</v>
       </c>
       <c r="M295" s="91">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>637535.33849999995</v>
       </c>
     </row>
@@ -8515,14 +8517,14 @@
       <c r="A318" s="126" t="s">
         <v>155</v>
       </c>
-      <c r="B318" s="160" t="s">
+      <c r="B318" s="157" t="s">
         <v>227</v>
       </c>
       <c r="D318" s="129" t="s">
         <v>230</v>
       </c>
       <c r="E318" s="127"/>
-      <c r="F318" s="160" t="s">
+      <c r="F318" s="157" t="s">
         <v>227</v>
       </c>
     </row>
@@ -8531,23 +8533,23 @@
         <v>156</v>
       </c>
       <c r="B319" s="128"/>
-      <c r="D319" s="159" t="s">
+      <c r="D319" s="175" t="s">
         <v>161</v>
       </c>
-      <c r="E319" s="159"/>
+      <c r="E319" s="175"/>
       <c r="F319" s="71"/>
     </row>
     <row r="320" spans="1:14">
-      <c r="A320" s="161" t="s">
+      <c r="A320" s="158" t="s">
         <v>157</v>
       </c>
       <c r="B320" s="125">
         <v>87000</v>
       </c>
-      <c r="D320" s="162" t="s">
+      <c r="D320" s="171" t="s">
         <v>157</v>
       </c>
-      <c r="E320" s="162"/>
+      <c r="E320" s="171"/>
       <c r="F320" s="127">
         <v>120000</v>
       </c>
@@ -8559,27 +8561,27 @@
       <c r="B321" s="125">
         <v>20000</v>
       </c>
-      <c r="D321" s="157" t="s">
+      <c r="D321" s="172" t="s">
         <v>162</v>
       </c>
-      <c r="E321" s="163"/>
-      <c r="F321" s="158"/>
+      <c r="E321" s="173"/>
+      <c r="F321" s="174"/>
     </row>
     <row r="322" spans="1:14">
       <c r="A322" s="125" t="s">
         <v>159</v>
       </c>
       <c r="B322" s="125"/>
-      <c r="D322" s="162" t="s">
+      <c r="D322" s="171" t="s">
         <v>163</v>
       </c>
-      <c r="E322" s="162"/>
+      <c r="E322" s="171"/>
       <c r="F322" s="130">
         <v>0.05</v>
       </c>
     </row>
     <row r="323" spans="1:14">
-      <c r="A323" s="161" t="s">
+      <c r="A323" s="158" t="s">
         <v>160</v>
       </c>
       <c r="B323" s="125">
@@ -8673,7 +8675,7 @@
         <v>87000</v>
       </c>
       <c r="N327" s="134">
-        <f t="shared" ref="N327:N328" si="54">SUM(B327:M327)</f>
+        <f t="shared" ref="N327:N328" si="56">SUM(B327:M327)</f>
         <v>1104000</v>
       </c>
     </row>
@@ -8718,7 +8720,7 @@
         <v>147000</v>
       </c>
       <c r="N328" s="134">
-        <f t="shared" si="54"/>
+        <f t="shared" si="56"/>
         <v>1764000</v>
       </c>
     </row>
@@ -8731,51 +8733,51 @@
         <v>254000</v>
       </c>
       <c r="C329" s="136">
-        <f t="shared" ref="C329:N329" si="55">SUM(C327:C328)</f>
+        <f t="shared" ref="C329:N329" si="57">SUM(C327:C328)</f>
         <v>254000</v>
       </c>
       <c r="D329" s="136">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>254000</v>
       </c>
       <c r="E329" s="136">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>234000</v>
       </c>
       <c r="F329" s="136">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>234000</v>
       </c>
       <c r="G329" s="136">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>234000</v>
       </c>
       <c r="H329" s="136">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>234000</v>
       </c>
       <c r="I329" s="136">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>234000</v>
       </c>
       <c r="J329" s="136">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>234000</v>
       </c>
       <c r="K329" s="136">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>234000</v>
       </c>
       <c r="L329" s="136">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>234000</v>
       </c>
       <c r="M329" s="136">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>234000</v>
       </c>
       <c r="N329" s="136">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>2868000</v>
       </c>
     </row>
@@ -8833,27 +8835,27 @@
         <v>117857.25</v>
       </c>
       <c r="C331" s="137">
-        <f>F120*0.05</f>
+        <f t="shared" ref="C331:H331" si="58">F120*0.05</f>
         <v>129599.5</v>
       </c>
       <c r="D331" s="137">
-        <f>G120*0.05</f>
+        <f t="shared" si="58"/>
         <v>136439</v>
       </c>
       <c r="E331" s="137">
-        <f>H120*0.05</f>
+        <f t="shared" si="58"/>
         <v>125265.75</v>
       </c>
       <c r="F331" s="137">
-        <f>I120*0.05</f>
+        <f t="shared" si="58"/>
         <v>144122.25</v>
       </c>
       <c r="G331" s="137">
-        <f>J120*0.05</f>
+        <f t="shared" si="58"/>
         <v>171944.75</v>
       </c>
       <c r="H331" s="137">
-        <f>K120*0.05</f>
+        <f t="shared" si="58"/>
         <v>171541.5</v>
       </c>
       <c r="I331" s="137">
@@ -8890,51 +8892,51 @@
         <v>237857.25</v>
       </c>
       <c r="C332" s="139">
-        <f t="shared" ref="C332:N332" si="56">SUM(C330:C331)</f>
+        <f t="shared" ref="C332:N332" si="59">SUM(C330:C331)</f>
         <v>249599.5</v>
       </c>
       <c r="D332" s="139">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>256439</v>
       </c>
       <c r="E332" s="139">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>245265.75</v>
       </c>
       <c r="F332" s="139">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>264122.25</v>
       </c>
       <c r="G332" s="139">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>291944.75</v>
       </c>
       <c r="H332" s="139">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>291541.5</v>
       </c>
       <c r="I332" s="139">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>274698.63750000001</v>
       </c>
       <c r="J332" s="139">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>250663.41750000001</v>
       </c>
       <c r="K332" s="139">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>238267.6275</v>
       </c>
       <c r="L332" s="139">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>237857.25</v>
       </c>
       <c r="M332" s="139">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>239152</v>
       </c>
       <c r="N332" s="139">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>3077408.9325000001</v>
       </c>
     </row>
@@ -8947,51 +8949,51 @@
         <v>491857.25</v>
       </c>
       <c r="C333" s="141">
-        <f t="shared" ref="C333:N333" si="57">C332+C329</f>
+        <f t="shared" ref="C333:N333" si="60">C332+C329</f>
         <v>503599.5</v>
       </c>
       <c r="D333" s="141">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>510439</v>
       </c>
       <c r="E333" s="141">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>479265.75</v>
       </c>
       <c r="F333" s="141">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>498122.25</v>
       </c>
       <c r="G333" s="141">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>525944.75</v>
       </c>
       <c r="H333" s="141">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>525541.5</v>
       </c>
       <c r="I333" s="141">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>508698.63750000001</v>
       </c>
       <c r="J333" s="141">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>484663.41749999998</v>
       </c>
       <c r="K333" s="141">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>472267.6275</v>
       </c>
       <c r="L333" s="141">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>471857.25</v>
       </c>
       <c r="M333" s="141">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>473152</v>
       </c>
       <c r="N333" s="141">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>5945408.9325000001</v>
       </c>
     </row>
@@ -9053,47 +9055,47 @@
         <v>2357145</v>
       </c>
       <c r="C340" s="93">
-        <f t="shared" ref="C340:M340" si="58">D120</f>
+        <f t="shared" ref="C340:M340" si="61">D120</f>
         <v>2383040</v>
       </c>
       <c r="D340" s="93">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>2747720</v>
       </c>
       <c r="E340" s="93">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>2591990</v>
       </c>
       <c r="F340" s="93">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>2728780</v>
       </c>
       <c r="G340" s="93">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>2505315</v>
       </c>
       <c r="H340" s="93">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>2882445</v>
       </c>
       <c r="I340" s="93">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>3438895</v>
       </c>
       <c r="J340" s="93">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>3430830</v>
       </c>
       <c r="K340" s="93">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>3125225</v>
       </c>
       <c r="L340" s="93">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>2639665</v>
       </c>
       <c r="M340" s="93">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>2389245</v>
       </c>
       <c r="N340" s="93">
@@ -9110,51 +9112,51 @@
         <v>627240.6</v>
       </c>
       <c r="C341" s="94">
-        <f t="shared" ref="C341:M341" si="59">C295</f>
+        <f t="shared" ref="C341:M341" si="62">C295</f>
         <v>654896.60000000009</v>
       </c>
       <c r="D341" s="94">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>713276.4</v>
       </c>
       <c r="E341" s="94">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>694730.6</v>
       </c>
       <c r="F341" s="94">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>705826.39999999991</v>
       </c>
       <c r="G341" s="94">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>692302.8</v>
       </c>
       <c r="H341" s="94">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>804488.4</v>
       </c>
       <c r="I341" s="94">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>901952.2</v>
       </c>
       <c r="J341" s="94">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>877510.59999999986</v>
       </c>
       <c r="K341" s="94">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>784366.4</v>
       </c>
       <c r="L341" s="94">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>680190.57000000007</v>
       </c>
       <c r="M341" s="94">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>637535.33849999995</v>
       </c>
       <c r="N341" s="94">
-        <f t="shared" ref="N341:N348" si="60">SUM(B341:M341)</f>
+        <f t="shared" ref="N341:N348" si="63">SUM(B341:M341)</f>
         <v>8774316.9085000008</v>
       </c>
     </row>
@@ -9167,51 +9169,51 @@
         <v>130834.53672727273</v>
       </c>
       <c r="C342" s="95">
-        <f t="shared" ref="C342:M342" si="61">C277</f>
+        <f t="shared" ref="C342:M342" si="64">C277</f>
         <v>131458.432</v>
       </c>
       <c r="D342" s="95">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>135223.37163636362</v>
       </c>
       <c r="E342" s="95">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>135961.02981818182</v>
       </c>
       <c r="F342" s="95">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>135871.36290909088</v>
       </c>
       <c r="G342" s="95">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>133761.95200000002</v>
       </c>
       <c r="H342" s="95">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>144814.71127272726</v>
       </c>
       <c r="I342" s="95">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>176512.83025454549</v>
       </c>
       <c r="J342" s="95">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>170918.73919999998</v>
       </c>
       <c r="K342" s="95">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>139238.92072727272</v>
       </c>
       <c r="L342" s="95">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>135322.57454545458</v>
       </c>
       <c r="M342" s="95">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>130378.0821818182</v>
       </c>
       <c r="N342" s="95">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>1700296.5432727272</v>
       </c>
     </row>
@@ -9220,55 +9222,55 @@
         <v>228</v>
       </c>
       <c r="B343" s="96">
-        <f t="shared" ref="B343" si="62">B340-B341-B342</f>
+        <f t="shared" ref="B343" si="65">B340-B341-B342</f>
         <v>1599069.8632727272</v>
       </c>
       <c r="C343" s="96">
-        <f t="shared" ref="C343" si="63">C340-C341-C342</f>
+        <f t="shared" ref="C343" si="66">C340-C341-C342</f>
         <v>1596684.9679999999</v>
       </c>
       <c r="D343" s="96">
-        <f t="shared" ref="D343" si="64">D340-D341-D342</f>
+        <f t="shared" ref="D343" si="67">D340-D341-D342</f>
         <v>1899220.2283636364</v>
       </c>
       <c r="E343" s="96">
-        <f t="shared" ref="E343" si="65">E340-E341-E342</f>
+        <f t="shared" ref="E343" si="68">E340-E341-E342</f>
         <v>1761298.370181818</v>
       </c>
       <c r="F343" s="96">
-        <f t="shared" ref="F343" si="66">F340-F341-F342</f>
+        <f t="shared" ref="F343" si="69">F340-F341-F342</f>
         <v>1887082.2370909092</v>
       </c>
       <c r="G343" s="96">
-        <f t="shared" ref="G343" si="67">G340-G341-G342</f>
+        <f t="shared" ref="G343" si="70">G340-G341-G342</f>
         <v>1679250.2479999999</v>
       </c>
       <c r="H343" s="96">
-        <f t="shared" ref="H343" si="68">H340-H341-H342</f>
+        <f t="shared" ref="H343" si="71">H340-H341-H342</f>
         <v>1933141.8887272729</v>
       </c>
       <c r="I343" s="96">
-        <f t="shared" ref="I343" si="69">I340-I341-I342</f>
+        <f t="shared" ref="I343" si="72">I340-I341-I342</f>
         <v>2360429.9697454544</v>
       </c>
       <c r="J343" s="96">
-        <f t="shared" ref="J343" si="70">J340-J341-J342</f>
+        <f t="shared" ref="J343" si="73">J340-J341-J342</f>
         <v>2382400.6608000002</v>
       </c>
       <c r="K343" s="96">
-        <f t="shared" ref="K343" si="71">K340-K341-K342</f>
+        <f t="shared" ref="K343" si="74">K340-K341-K342</f>
         <v>2201619.6792727276</v>
       </c>
       <c r="L343" s="96">
-        <f t="shared" ref="L343" si="72">L340-L341-L342</f>
+        <f t="shared" ref="L343" si="75">L340-L341-L342</f>
         <v>1824151.8554545455</v>
       </c>
       <c r="M343" s="96">
-        <f t="shared" ref="M343" si="73">M340-M341-M342</f>
+        <f t="shared" ref="M343" si="76">M340-M341-M342</f>
         <v>1621331.5793181816</v>
       </c>
       <c r="N343" s="96">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>22745681.548227269</v>
       </c>
     </row>
@@ -9281,51 +9283,51 @@
         <v>491857.25</v>
       </c>
       <c r="C344" s="94">
-        <f t="shared" ref="C344:M344" si="74">C333</f>
+        <f t="shared" ref="C344:M344" si="77">C333</f>
         <v>503599.5</v>
       </c>
       <c r="D344" s="94">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>510439</v>
       </c>
       <c r="E344" s="94">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>479265.75</v>
       </c>
       <c r="F344" s="94">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>498122.25</v>
       </c>
       <c r="G344" s="94">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>525944.75</v>
       </c>
       <c r="H344" s="94">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>525541.5</v>
       </c>
       <c r="I344" s="94">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>508698.63750000001</v>
       </c>
       <c r="J344" s="94">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>484663.41749999998</v>
       </c>
       <c r="K344" s="94">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>472267.6275</v>
       </c>
       <c r="L344" s="94">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>471857.25</v>
       </c>
       <c r="M344" s="94">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>473152</v>
       </c>
       <c r="N344" s="94">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>5945408.9325000001</v>
       </c>
     </row>
@@ -9370,7 +9372,7 @@
         <v>6678</v>
       </c>
       <c r="N345" s="95">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>80070</v>
       </c>
     </row>
@@ -9379,55 +9381,55 @@
         <v>171</v>
       </c>
       <c r="B346" s="96">
-        <f t="shared" ref="B346" si="75">B343-B344-B345</f>
+        <f t="shared" ref="B346" si="78">B343-B344-B345</f>
         <v>1100545.6132727272</v>
       </c>
       <c r="C346" s="96">
-        <f t="shared" ref="C346" si="76">C343-C344-C345</f>
+        <f t="shared" ref="C346" si="79">C343-C344-C345</f>
         <v>1086417.4679999999</v>
       </c>
       <c r="D346" s="96">
-        <f t="shared" ref="D346" si="77">D343-D344-D345</f>
+        <f t="shared" ref="D346" si="80">D343-D344-D345</f>
         <v>1382112.2283636364</v>
       </c>
       <c r="E346" s="96">
-        <f t="shared" ref="E346" si="78">E343-E344-E345</f>
+        <f t="shared" ref="E346" si="81">E343-E344-E345</f>
         <v>1275362.620181818</v>
       </c>
       <c r="F346" s="96">
-        <f t="shared" ref="F346" si="79">F343-F344-F345</f>
+        <f t="shared" ref="F346" si="82">F343-F344-F345</f>
         <v>1382288.9870909092</v>
       </c>
       <c r="G346" s="96">
-        <f t="shared" ref="G346" si="80">G343-G344-G345</f>
+        <f t="shared" ref="G346" si="83">G343-G344-G345</f>
         <v>1146633.4979999999</v>
       </c>
       <c r="H346" s="96">
-        <f t="shared" ref="H346" si="81">H343-H344-H345</f>
+        <f t="shared" ref="H346" si="84">H343-H344-H345</f>
         <v>1400927.3887272729</v>
       </c>
       <c r="I346" s="96">
-        <f t="shared" ref="I346" si="82">I343-I344-I345</f>
+        <f t="shared" ref="I346" si="85">I343-I344-I345</f>
         <v>1845057.3322454544</v>
       </c>
       <c r="J346" s="96">
-        <f t="shared" ref="J346" si="83">J343-J344-J345</f>
+        <f t="shared" ref="J346" si="86">J343-J344-J345</f>
         <v>1891062.2433000002</v>
       </c>
       <c r="K346" s="96">
-        <f t="shared" ref="K346" si="84">K343-K344-K345</f>
+        <f t="shared" ref="K346" si="87">K343-K344-K345</f>
         <v>1722676.0517727276</v>
       </c>
       <c r="L346" s="96">
-        <f t="shared" ref="L346" si="85">L343-L344-L345</f>
+        <f t="shared" ref="L346" si="88">L343-L344-L345</f>
         <v>1345617.6054545455</v>
       </c>
       <c r="M346" s="96">
-        <f t="shared" ref="M346" si="86">M343-M344-M345</f>
+        <f t="shared" ref="M346" si="89">M343-M344-M345</f>
         <v>1141501.5793181816</v>
       </c>
       <c r="N346" s="96">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>16720202.615727272</v>
       </c>
     </row>
@@ -9440,51 +9442,51 @@
         <v>385190.96464545449</v>
       </c>
       <c r="C347" s="95">
-        <f t="shared" ref="C347:M347" si="87">C346*0.35</f>
+        <f t="shared" ref="C347:M347" si="90">C346*0.35</f>
         <v>380246.11379999993</v>
       </c>
       <c r="D347" s="95">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>483739.2799272727</v>
       </c>
       <c r="E347" s="95">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>446376.9170636363</v>
       </c>
       <c r="F347" s="95">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>483801.14548181818</v>
       </c>
       <c r="G347" s="95">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>401321.72429999994</v>
       </c>
       <c r="H347" s="95">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>490324.58605454548</v>
       </c>
       <c r="I347" s="95">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>645770.06628590904</v>
       </c>
       <c r="J347" s="95">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>661871.78515500005</v>
       </c>
       <c r="K347" s="95">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>602936.6181204546</v>
       </c>
       <c r="L347" s="95">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>470966.16190909088</v>
       </c>
       <c r="M347" s="95">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>399525.55276136356</v>
       </c>
       <c r="N347" s="95">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>5852070.915504545</v>
       </c>
     </row>
@@ -9497,100 +9499,100 @@
         <v>715354.64862727281</v>
       </c>
       <c r="C348" s="92">
-        <f t="shared" ref="C348:M348" si="88">C346-C347</f>
+        <f t="shared" ref="C348:M348" si="91">C346-C347</f>
         <v>706171.35419999994</v>
       </c>
       <c r="D348" s="92">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>898372.94843636372</v>
       </c>
       <c r="E348" s="92">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>828985.70311818179</v>
       </c>
       <c r="F348" s="92">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>898487.84160909103</v>
       </c>
       <c r="G348" s="92">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>745311.77370000002</v>
       </c>
       <c r="H348" s="92">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>910602.80267272738</v>
       </c>
       <c r="I348" s="92">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>1199287.2659595455</v>
       </c>
       <c r="J348" s="92">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>1229190.458145</v>
       </c>
       <c r="K348" s="92">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>1119739.4336522729</v>
       </c>
       <c r="L348" s="92">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>874651.44354545465</v>
       </c>
       <c r="M348" s="92">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>741976.02655681805</v>
       </c>
       <c r="N348" s="92">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>10868131.700222727</v>
       </c>
     </row>
     <row r="349" spans="1:14" s="8" customFormat="1">
-      <c r="A349" s="167"/>
-      <c r="B349" s="168"/>
-      <c r="C349" s="168"/>
-      <c r="D349" s="168"/>
-      <c r="E349" s="168"/>
-      <c r="F349" s="168"/>
-      <c r="G349" s="168"/>
-      <c r="H349" s="168"/>
-      <c r="I349" s="168"/>
-      <c r="J349" s="168"/>
-      <c r="K349" s="168"/>
-      <c r="L349" s="168"/>
-      <c r="M349" s="168"/>
+      <c r="A349" s="162"/>
+      <c r="B349" s="163"/>
+      <c r="C349" s="163"/>
+      <c r="D349" s="163"/>
+      <c r="E349" s="163"/>
+      <c r="F349" s="163"/>
+      <c r="G349" s="163"/>
+      <c r="H349" s="163"/>
+      <c r="I349" s="163"/>
+      <c r="J349" s="163"/>
+      <c r="K349" s="163"/>
+      <c r="L349" s="163"/>
+      <c r="M349" s="163"/>
     </row>
     <row r="350" spans="1:14" s="8" customFormat="1">
-      <c r="A350" s="167"/>
-      <c r="B350" s="168"/>
-      <c r="C350" s="168"/>
-      <c r="D350" s="168"/>
-      <c r="E350" s="168"/>
-      <c r="F350" s="168"/>
-      <c r="G350" s="168"/>
-      <c r="H350" s="168"/>
-      <c r="I350" s="168"/>
-      <c r="J350" s="168"/>
-      <c r="K350" s="168"/>
-      <c r="L350" s="168"/>
-      <c r="M350" s="168"/>
+      <c r="A350" s="162"/>
+      <c r="B350" s="163"/>
+      <c r="C350" s="163"/>
+      <c r="D350" s="163"/>
+      <c r="E350" s="163"/>
+      <c r="F350" s="163"/>
+      <c r="G350" s="163"/>
+      <c r="H350" s="163"/>
+      <c r="I350" s="163"/>
+      <c r="J350" s="163"/>
+      <c r="K350" s="163"/>
+      <c r="L350" s="163"/>
+      <c r="M350" s="163"/>
     </row>
     <row r="351" spans="1:14" s="8" customFormat="1" ht="18.75">
       <c r="A351" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="B351" s="168"/>
-      <c r="C351" s="168"/>
-      <c r="D351" s="168"/>
-      <c r="E351" s="168"/>
-      <c r="F351" s="168"/>
-      <c r="G351" s="168"/>
-      <c r="H351" s="168"/>
-      <c r="I351" s="168"/>
-      <c r="J351" s="168"/>
-      <c r="K351" s="168"/>
-      <c r="L351" s="168"/>
-      <c r="M351" s="168"/>
+      <c r="B351" s="163"/>
+      <c r="C351" s="163"/>
+      <c r="D351" s="163"/>
+      <c r="E351" s="163"/>
+      <c r="F351" s="163"/>
+      <c r="G351" s="163"/>
+      <c r="H351" s="163"/>
+      <c r="I351" s="163"/>
+      <c r="J351" s="163"/>
+      <c r="K351" s="163"/>
+      <c r="L351" s="163"/>
+      <c r="M351" s="163"/>
     </row>
     <row r="352" spans="1:14" s="8" customFormat="1">
       <c r="A352" s="155" t="s">
@@ -9599,17 +9601,17 @@
       <c r="B352" s="99" t="s">
         <v>206</v>
       </c>
-      <c r="C352" s="168"/>
-      <c r="D352" s="168"/>
-      <c r="E352" s="168"/>
-      <c r="F352" s="168"/>
-      <c r="G352" s="168"/>
-      <c r="H352" s="168"/>
-      <c r="I352" s="168"/>
-      <c r="J352" s="168"/>
-      <c r="K352" s="168"/>
-      <c r="L352" s="168"/>
-      <c r="M352" s="168"/>
+      <c r="C352" s="163"/>
+      <c r="D352" s="163"/>
+      <c r="E352" s="163"/>
+      <c r="F352" s="163"/>
+      <c r="G352" s="163"/>
+      <c r="H352" s="163"/>
+      <c r="I352" s="163"/>
+      <c r="J352" s="163"/>
+      <c r="K352" s="163"/>
+      <c r="L352" s="163"/>
+      <c r="M352" s="163"/>
     </row>
     <row r="353" spans="1:14" s="8" customFormat="1">
       <c r="A353" s="71" t="s">
@@ -9618,17 +9620,17 @@
       <c r="B353" s="93">
         <v>33220295</v>
       </c>
-      <c r="C353" s="168"/>
-      <c r="D353" s="168"/>
-      <c r="E353" s="168"/>
-      <c r="F353" s="168"/>
-      <c r="G353" s="168"/>
-      <c r="H353" s="168"/>
-      <c r="I353" s="168"/>
-      <c r="J353" s="168"/>
-      <c r="K353" s="168"/>
-      <c r="L353" s="168"/>
-      <c r="M353" s="168"/>
+      <c r="C353" s="163"/>
+      <c r="D353" s="163"/>
+      <c r="E353" s="163"/>
+      <c r="F353" s="163"/>
+      <c r="G353" s="163"/>
+      <c r="H353" s="163"/>
+      <c r="I353" s="163"/>
+      <c r="J353" s="163"/>
+      <c r="K353" s="163"/>
+      <c r="L353" s="163"/>
+      <c r="M353" s="163"/>
     </row>
     <row r="354" spans="1:14" s="8" customFormat="1">
       <c r="A354" s="71" t="s">
@@ -9637,17 +9639,17 @@
       <c r="B354" s="94">
         <v>8774316.9085000008</v>
       </c>
-      <c r="C354" s="168"/>
-      <c r="D354" s="168"/>
-      <c r="E354" s="168"/>
-      <c r="F354" s="168"/>
-      <c r="G354" s="168"/>
-      <c r="H354" s="168"/>
-      <c r="I354" s="168"/>
-      <c r="J354" s="168"/>
-      <c r="K354" s="168"/>
-      <c r="L354" s="168"/>
-      <c r="M354" s="168"/>
+      <c r="C354" s="163"/>
+      <c r="D354" s="163"/>
+      <c r="E354" s="163"/>
+      <c r="F354" s="163"/>
+      <c r="G354" s="163"/>
+      <c r="H354" s="163"/>
+      <c r="I354" s="163"/>
+      <c r="J354" s="163"/>
+      <c r="K354" s="163"/>
+      <c r="L354" s="163"/>
+      <c r="M354" s="163"/>
     </row>
     <row r="355" spans="1:14" s="8" customFormat="1" ht="15.75" thickBot="1">
       <c r="A355" s="71" t="s">
@@ -9656,17 +9658,17 @@
       <c r="B355" s="95">
         <v>1700296.5432727272</v>
       </c>
-      <c r="C355" s="168"/>
-      <c r="D355" s="168"/>
-      <c r="E355" s="168"/>
-      <c r="F355" s="168"/>
-      <c r="G355" s="168"/>
-      <c r="H355" s="168"/>
-      <c r="I355" s="168"/>
-      <c r="J355" s="168"/>
-      <c r="K355" s="168"/>
-      <c r="L355" s="168"/>
-      <c r="M355" s="168"/>
+      <c r="C355" s="163"/>
+      <c r="D355" s="163"/>
+      <c r="E355" s="163"/>
+      <c r="F355" s="163"/>
+      <c r="G355" s="163"/>
+      <c r="H355" s="163"/>
+      <c r="I355" s="163"/>
+      <c r="J355" s="163"/>
+      <c r="K355" s="163"/>
+      <c r="L355" s="163"/>
+      <c r="M355" s="163"/>
     </row>
     <row r="356" spans="1:14" s="8" customFormat="1">
       <c r="A356" s="98" t="s">
@@ -9675,17 +9677,17 @@
       <c r="B356" s="96">
         <v>22745681.548227269</v>
       </c>
-      <c r="C356" s="168"/>
-      <c r="D356" s="168"/>
-      <c r="E356" s="168"/>
-      <c r="F356" s="168"/>
-      <c r="G356" s="168"/>
-      <c r="H356" s="168"/>
-      <c r="I356" s="168"/>
-      <c r="J356" s="168"/>
-      <c r="K356" s="168"/>
-      <c r="L356" s="168"/>
-      <c r="M356" s="168"/>
+      <c r="C356" s="163"/>
+      <c r="D356" s="163"/>
+      <c r="E356" s="163"/>
+      <c r="F356" s="163"/>
+      <c r="G356" s="163"/>
+      <c r="H356" s="163"/>
+      <c r="I356" s="163"/>
+      <c r="J356" s="163"/>
+      <c r="K356" s="163"/>
+      <c r="L356" s="163"/>
+      <c r="M356" s="163"/>
     </row>
     <row r="357" spans="1:14" s="8" customFormat="1">
       <c r="A357" s="71" t="s">
@@ -9694,17 +9696,17 @@
       <c r="B357" s="94">
         <v>5945408.9325000001</v>
       </c>
-      <c r="C357" s="168"/>
-      <c r="D357" s="168"/>
-      <c r="E357" s="168"/>
-      <c r="F357" s="168"/>
-      <c r="G357" s="168"/>
-      <c r="H357" s="168"/>
-      <c r="I357" s="168"/>
-      <c r="J357" s="168"/>
-      <c r="K357" s="168"/>
-      <c r="L357" s="168"/>
-      <c r="M357" s="168"/>
+      <c r="C357" s="163"/>
+      <c r="D357" s="163"/>
+      <c r="E357" s="163"/>
+      <c r="F357" s="163"/>
+      <c r="G357" s="163"/>
+      <c r="H357" s="163"/>
+      <c r="I357" s="163"/>
+      <c r="J357" s="163"/>
+      <c r="K357" s="163"/>
+      <c r="L357" s="163"/>
+      <c r="M357" s="163"/>
     </row>
     <row r="358" spans="1:14" s="8" customFormat="1" ht="15.75" thickBot="1">
       <c r="A358" s="71" t="s">
@@ -9713,17 +9715,17 @@
       <c r="B358" s="95">
         <v>80070</v>
       </c>
-      <c r="C358" s="168"/>
-      <c r="D358" s="168"/>
-      <c r="E358" s="168"/>
-      <c r="F358" s="168"/>
-      <c r="G358" s="168"/>
-      <c r="H358" s="168"/>
-      <c r="I358" s="168"/>
-      <c r="J358" s="168"/>
-      <c r="K358" s="168"/>
-      <c r="L358" s="168"/>
-      <c r="M358" s="168"/>
+      <c r="C358" s="163"/>
+      <c r="D358" s="163"/>
+      <c r="E358" s="163"/>
+      <c r="F358" s="163"/>
+      <c r="G358" s="163"/>
+      <c r="H358" s="163"/>
+      <c r="I358" s="163"/>
+      <c r="J358" s="163"/>
+      <c r="K358" s="163"/>
+      <c r="L358" s="163"/>
+      <c r="M358" s="163"/>
     </row>
     <row r="359" spans="1:14" s="8" customFormat="1">
       <c r="A359" s="98" t="s">
@@ -9732,17 +9734,17 @@
       <c r="B359" s="96">
         <v>16720202.615727272</v>
       </c>
-      <c r="C359" s="168"/>
-      <c r="D359" s="168"/>
-      <c r="E359" s="168"/>
-      <c r="F359" s="168"/>
-      <c r="G359" s="168"/>
-      <c r="H359" s="168"/>
-      <c r="I359" s="168"/>
-      <c r="J359" s="168"/>
-      <c r="K359" s="168"/>
-      <c r="L359" s="168"/>
-      <c r="M359" s="168"/>
+      <c r="C359" s="163"/>
+      <c r="D359" s="163"/>
+      <c r="E359" s="163"/>
+      <c r="F359" s="163"/>
+      <c r="G359" s="163"/>
+      <c r="H359" s="163"/>
+      <c r="I359" s="163"/>
+      <c r="J359" s="163"/>
+      <c r="K359" s="163"/>
+      <c r="L359" s="163"/>
+      <c r="M359" s="163"/>
     </row>
     <row r="360" spans="1:14" s="8" customFormat="1" ht="15.75" thickBot="1">
       <c r="A360" s="71" t="s">
@@ -9751,17 +9753,17 @@
       <c r="B360" s="95">
         <v>5852070.915504545</v>
       </c>
-      <c r="C360" s="168"/>
-      <c r="D360" s="168"/>
-      <c r="E360" s="168"/>
-      <c r="F360" s="168"/>
-      <c r="G360" s="168"/>
-      <c r="H360" s="168"/>
-      <c r="I360" s="168"/>
-      <c r="J360" s="168"/>
-      <c r="K360" s="168"/>
-      <c r="L360" s="168"/>
-      <c r="M360" s="168"/>
+      <c r="C360" s="163"/>
+      <c r="D360" s="163"/>
+      <c r="E360" s="163"/>
+      <c r="F360" s="163"/>
+      <c r="G360" s="163"/>
+      <c r="H360" s="163"/>
+      <c r="I360" s="163"/>
+      <c r="J360" s="163"/>
+      <c r="K360" s="163"/>
+      <c r="L360" s="163"/>
+      <c r="M360" s="163"/>
     </row>
     <row r="361" spans="1:14" s="8" customFormat="1">
       <c r="A361" s="81" t="s">
@@ -9770,31 +9772,31 @@
       <c r="B361" s="92">
         <v>10868131.700222727</v>
       </c>
-      <c r="C361" s="168"/>
-      <c r="D361" s="168"/>
-      <c r="E361" s="168"/>
-      <c r="F361" s="168"/>
-      <c r="G361" s="168"/>
-      <c r="H361" s="168"/>
-      <c r="I361" s="168"/>
-      <c r="J361" s="168"/>
-      <c r="K361" s="168"/>
-      <c r="L361" s="168"/>
-      <c r="M361" s="168"/>
+      <c r="C361" s="163"/>
+      <c r="D361" s="163"/>
+      <c r="E361" s="163"/>
+      <c r="F361" s="163"/>
+      <c r="G361" s="163"/>
+      <c r="H361" s="163"/>
+      <c r="I361" s="163"/>
+      <c r="J361" s="163"/>
+      <c r="K361" s="163"/>
+      <c r="L361" s="163"/>
+      <c r="M361" s="163"/>
     </row>
     <row r="362" spans="1:14" s="8" customFormat="1">
-      <c r="A362" s="167"/>
-      <c r="C362" s="168"/>
-      <c r="D362" s="168"/>
-      <c r="E362" s="168"/>
-      <c r="F362" s="168"/>
-      <c r="G362" s="168"/>
-      <c r="H362" s="168"/>
-      <c r="I362" s="168"/>
-      <c r="J362" s="168"/>
-      <c r="K362" s="168"/>
-      <c r="L362" s="168"/>
-      <c r="M362" s="168"/>
+      <c r="A362" s="162"/>
+      <c r="C362" s="163"/>
+      <c r="D362" s="163"/>
+      <c r="E362" s="163"/>
+      <c r="F362" s="163"/>
+      <c r="G362" s="163"/>
+      <c r="H362" s="163"/>
+      <c r="I362" s="163"/>
+      <c r="J362" s="163"/>
+      <c r="K362" s="163"/>
+      <c r="L362" s="163"/>
+      <c r="M362" s="163"/>
     </row>
     <row r="363" spans="1:14" ht="26.25">
       <c r="A363" s="30" t="s">
@@ -9846,7 +9848,7 @@
       </c>
     </row>
     <row r="366" spans="1:14">
-      <c r="A366" s="173" t="s">
+      <c r="A366" s="168" t="s">
         <v>174</v>
       </c>
       <c r="B366" s="101">
@@ -9854,47 +9856,47 @@
         <v>2269716.2731237495</v>
       </c>
       <c r="C366" s="101">
-        <f t="shared" ref="C366:M366" si="89">D145</f>
+        <f t="shared" ref="C366:M366" si="92">D145</f>
         <v>2325274.0508249998</v>
       </c>
       <c r="D366" s="101">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>2516868.6641999995</v>
       </c>
       <c r="E366" s="101">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>2619368.0419499995</v>
       </c>
       <c r="F366" s="101">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>2610077.1196499998</v>
       </c>
       <c r="G366" s="101">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>2567559.1317750001</v>
       </c>
       <c r="H366" s="101">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>2642938.7291999999</v>
       </c>
       <c r="I366" s="101">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>3100901.7302999999</v>
       </c>
       <c r="J366" s="101">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>3369909.2501249998</v>
       </c>
       <c r="K366" s="101">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>3216039.999975</v>
       </c>
       <c r="L366" s="101">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>2827937.9650499998</v>
       </c>
       <c r="M366" s="101">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>2466906.6559499996</v>
       </c>
       <c r="N366" s="101">
@@ -9924,56 +9926,56 @@
       <c r="A368" s="132" t="s">
         <v>217</v>
       </c>
-      <c r="B368" s="169">
+      <c r="B368" s="164">
         <f>B333</f>
         <v>491857.25</v>
       </c>
-      <c r="C368" s="169">
-        <f t="shared" ref="C368:M368" si="90">C333</f>
+      <c r="C368" s="164">
+        <f t="shared" ref="C368:M368" si="93">C333</f>
         <v>503599.5</v>
       </c>
-      <c r="D368" s="169">
-        <f t="shared" si="90"/>
+      <c r="D368" s="164">
+        <f t="shared" si="93"/>
         <v>510439</v>
       </c>
-      <c r="E368" s="169">
-        <f t="shared" si="90"/>
+      <c r="E368" s="164">
+        <f t="shared" si="93"/>
         <v>479265.75</v>
       </c>
-      <c r="F368" s="169">
-        <f t="shared" si="90"/>
+      <c r="F368" s="164">
+        <f t="shared" si="93"/>
         <v>498122.25</v>
       </c>
-      <c r="G368" s="169">
-        <f t="shared" si="90"/>
+      <c r="G368" s="164">
+        <f t="shared" si="93"/>
         <v>525944.75</v>
       </c>
-      <c r="H368" s="169">
-        <f t="shared" si="90"/>
+      <c r="H368" s="164">
+        <f t="shared" si="93"/>
         <v>525541.5</v>
       </c>
-      <c r="I368" s="169">
-        <f t="shared" si="90"/>
+      <c r="I368" s="164">
+        <f t="shared" si="93"/>
         <v>508698.63750000001</v>
       </c>
-      <c r="J368" s="169">
-        <f t="shared" si="90"/>
+      <c r="J368" s="164">
+        <f t="shared" si="93"/>
         <v>484663.41749999998</v>
       </c>
-      <c r="K368" s="169">
-        <f t="shared" si="90"/>
+      <c r="K368" s="164">
+        <f t="shared" si="93"/>
         <v>472267.6275</v>
       </c>
-      <c r="L368" s="169">
-        <f t="shared" si="90"/>
+      <c r="L368" s="164">
+        <f t="shared" si="93"/>
         <v>471857.25</v>
       </c>
-      <c r="M368" s="169">
-        <f t="shared" si="90"/>
+      <c r="M368" s="164">
+        <f t="shared" si="93"/>
         <v>473152</v>
       </c>
-      <c r="N368" s="169">
-        <f t="shared" ref="N368:N376" si="91">SUM(B368:M368)</f>
+      <c r="N368" s="164">
+        <f t="shared" ref="N368:N376" si="94">SUM(B368:M368)</f>
         <v>5945408.9325000001</v>
       </c>
     </row>
@@ -9981,56 +9983,56 @@
       <c r="A369" s="132" t="s">
         <v>218</v>
       </c>
-      <c r="B369" s="169">
+      <c r="B369" s="164">
         <f>B303</f>
         <v>0</v>
       </c>
-      <c r="C369" s="169">
-        <f t="shared" ref="C369:M369" si="92">C303</f>
+      <c r="C369" s="164">
+        <f t="shared" ref="C369:M369" si="95">C303</f>
         <v>0</v>
       </c>
-      <c r="D369" s="169">
-        <f t="shared" si="92"/>
+      <c r="D369" s="164">
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
-      <c r="E369" s="169">
-        <f t="shared" si="92"/>
+      <c r="E369" s="164">
+        <f t="shared" si="95"/>
         <v>190000</v>
       </c>
-      <c r="F369" s="169">
-        <f t="shared" si="92"/>
+      <c r="F369" s="164">
+        <f t="shared" si="95"/>
         <v>190000</v>
       </c>
-      <c r="G369" s="169">
-        <f t="shared" si="92"/>
+      <c r="G369" s="164">
+        <f t="shared" si="95"/>
         <v>190000</v>
       </c>
-      <c r="H369" s="169">
-        <f t="shared" si="92"/>
+      <c r="H369" s="164">
+        <f t="shared" si="95"/>
         <v>190000</v>
       </c>
-      <c r="I369" s="169">
-        <f t="shared" si="92"/>
+      <c r="I369" s="164">
+        <f t="shared" si="95"/>
         <v>190000</v>
       </c>
-      <c r="J369" s="169">
-        <f t="shared" si="92"/>
+      <c r="J369" s="164">
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
-      <c r="K369" s="169">
-        <f t="shared" si="92"/>
+      <c r="K369" s="164">
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
-      <c r="L369" s="169">
-        <f t="shared" si="92"/>
+      <c r="L369" s="164">
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
-      <c r="M369" s="169">
-        <f t="shared" si="92"/>
+      <c r="M369" s="164">
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
-      <c r="N369" s="169">
-        <f t="shared" si="91"/>
+      <c r="N369" s="164">
+        <f t="shared" si="94"/>
         <v>950000</v>
       </c>
     </row>
@@ -10038,56 +10040,56 @@
       <c r="A370" s="132" t="s">
         <v>128</v>
       </c>
-      <c r="B370" s="169">
+      <c r="B370" s="164">
         <f>B295</f>
         <v>627240.6</v>
       </c>
-      <c r="C370" s="169">
-        <f t="shared" ref="C370:M370" si="93">C295</f>
+      <c r="C370" s="164">
+        <f t="shared" ref="C370:M370" si="96">C295</f>
         <v>654896.60000000009</v>
       </c>
-      <c r="D370" s="169">
-        <f t="shared" si="93"/>
+      <c r="D370" s="164">
+        <f t="shared" si="96"/>
         <v>713276.4</v>
       </c>
-      <c r="E370" s="169">
-        <f t="shared" si="93"/>
+      <c r="E370" s="164">
+        <f t="shared" si="96"/>
         <v>694730.6</v>
       </c>
-      <c r="F370" s="169">
-        <f t="shared" si="93"/>
+      <c r="F370" s="164">
+        <f t="shared" si="96"/>
         <v>705826.39999999991</v>
       </c>
-      <c r="G370" s="169">
-        <f t="shared" si="93"/>
+      <c r="G370" s="164">
+        <f t="shared" si="96"/>
         <v>692302.8</v>
       </c>
-      <c r="H370" s="169">
-        <f t="shared" si="93"/>
+      <c r="H370" s="164">
+        <f t="shared" si="96"/>
         <v>804488.4</v>
       </c>
-      <c r="I370" s="169">
-        <f t="shared" si="93"/>
+      <c r="I370" s="164">
+        <f t="shared" si="96"/>
         <v>901952.2</v>
       </c>
-      <c r="J370" s="169">
-        <f t="shared" si="93"/>
+      <c r="J370" s="164">
+        <f t="shared" si="96"/>
         <v>877510.59999999986</v>
       </c>
-      <c r="K370" s="169">
-        <f t="shared" si="93"/>
+      <c r="K370" s="164">
+        <f t="shared" si="96"/>
         <v>784366.4</v>
       </c>
-      <c r="L370" s="169">
-        <f t="shared" si="93"/>
+      <c r="L370" s="164">
+        <f t="shared" si="96"/>
         <v>680190.57000000007</v>
       </c>
-      <c r="M370" s="169">
-        <f t="shared" si="93"/>
+      <c r="M370" s="164">
+        <f t="shared" si="96"/>
         <v>637535.33849999995</v>
       </c>
-      <c r="N370" s="169">
-        <f t="shared" si="91"/>
+      <c r="N370" s="164">
+        <f t="shared" si="94"/>
         <v>8774316.9085000008</v>
       </c>
     </row>
@@ -10095,56 +10097,56 @@
       <c r="A371" s="132" t="s">
         <v>167</v>
       </c>
-      <c r="B371" s="169">
+      <c r="B371" s="164">
         <f>B277</f>
         <v>130834.53672727273</v>
       </c>
-      <c r="C371" s="169">
-        <f t="shared" ref="C371:M371" si="94">C277</f>
+      <c r="C371" s="164">
+        <f t="shared" ref="C371:M371" si="97">C277</f>
         <v>131458.432</v>
       </c>
-      <c r="D371" s="169">
+      <c r="D371" s="164">
+        <f t="shared" si="97"/>
+        <v>135223.37163636362</v>
+      </c>
+      <c r="E371" s="164">
+        <f t="shared" si="97"/>
+        <v>135961.02981818182</v>
+      </c>
+      <c r="F371" s="164">
+        <f t="shared" si="97"/>
+        <v>135871.36290909088</v>
+      </c>
+      <c r="G371" s="164">
+        <f t="shared" si="97"/>
+        <v>133761.95200000002</v>
+      </c>
+      <c r="H371" s="164">
+        <f t="shared" si="97"/>
+        <v>144814.71127272726</v>
+      </c>
+      <c r="I371" s="164">
+        <f t="shared" si="97"/>
+        <v>176512.83025454549</v>
+      </c>
+      <c r="J371" s="164">
+        <f t="shared" si="97"/>
+        <v>170918.73919999998</v>
+      </c>
+      <c r="K371" s="164">
+        <f t="shared" si="97"/>
+        <v>139238.92072727272</v>
+      </c>
+      <c r="L371" s="164">
+        <f t="shared" si="97"/>
+        <v>135322.57454545458</v>
+      </c>
+      <c r="M371" s="164">
+        <f t="shared" si="97"/>
+        <v>130378.0821818182</v>
+      </c>
+      <c r="N371" s="164">
         <f t="shared" si="94"/>
-        <v>135223.37163636362</v>
-      </c>
-      <c r="E371" s="169">
-        <f t="shared" si="94"/>
-        <v>135961.02981818182</v>
-      </c>
-      <c r="F371" s="169">
-        <f t="shared" si="94"/>
-        <v>135871.36290909088</v>
-      </c>
-      <c r="G371" s="169">
-        <f t="shared" si="94"/>
-        <v>133761.95200000002</v>
-      </c>
-      <c r="H371" s="169">
-        <f t="shared" si="94"/>
-        <v>144814.71127272726</v>
-      </c>
-      <c r="I371" s="169">
-        <f t="shared" si="94"/>
-        <v>176512.83025454549</v>
-      </c>
-      <c r="J371" s="169">
-        <f t="shared" si="94"/>
-        <v>170918.73919999998</v>
-      </c>
-      <c r="K371" s="169">
-        <f t="shared" si="94"/>
-        <v>139238.92072727272</v>
-      </c>
-      <c r="L371" s="169">
-        <f t="shared" si="94"/>
-        <v>135322.57454545458</v>
-      </c>
-      <c r="M371" s="169">
-        <f t="shared" si="94"/>
-        <v>130378.0821818182</v>
-      </c>
-      <c r="N371" s="169">
-        <f t="shared" si="91"/>
         <v>1700296.5432727272</v>
       </c>
     </row>
@@ -10152,56 +10154,56 @@
       <c r="A372" s="132" t="s">
         <v>175</v>
       </c>
-      <c r="B372" s="169">
+      <c r="B372" s="164">
         <f>B347</f>
         <v>385190.96464545449</v>
       </c>
-      <c r="C372" s="169">
-        <f t="shared" ref="C372:M372" si="95">C347</f>
+      <c r="C372" s="164">
+        <f t="shared" ref="C372:M372" si="98">C347</f>
         <v>380246.11379999993</v>
       </c>
-      <c r="D372" s="169">
-        <f t="shared" si="95"/>
+      <c r="D372" s="164">
+        <f t="shared" si="98"/>
         <v>483739.2799272727</v>
       </c>
-      <c r="E372" s="169">
-        <f t="shared" si="95"/>
+      <c r="E372" s="164">
+        <f t="shared" si="98"/>
         <v>446376.9170636363</v>
       </c>
-      <c r="F372" s="169">
-        <f t="shared" si="95"/>
+      <c r="F372" s="164">
+        <f t="shared" si="98"/>
         <v>483801.14548181818</v>
       </c>
-      <c r="G372" s="169">
-        <f t="shared" si="95"/>
+      <c r="G372" s="164">
+        <f t="shared" si="98"/>
         <v>401321.72429999994</v>
       </c>
-      <c r="H372" s="169">
-        <f t="shared" si="95"/>
+      <c r="H372" s="164">
+        <f t="shared" si="98"/>
         <v>490324.58605454548</v>
       </c>
-      <c r="I372" s="169">
-        <f t="shared" si="95"/>
+      <c r="I372" s="164">
+        <f t="shared" si="98"/>
         <v>645770.06628590904</v>
       </c>
-      <c r="J372" s="169">
-        <f t="shared" si="95"/>
+      <c r="J372" s="164">
+        <f t="shared" si="98"/>
         <v>661871.78515500005</v>
       </c>
-      <c r="K372" s="169">
-        <f t="shared" si="95"/>
+      <c r="K372" s="164">
+        <f t="shared" si="98"/>
         <v>602936.6181204546</v>
       </c>
-      <c r="L372" s="169">
-        <f t="shared" si="95"/>
+      <c r="L372" s="164">
+        <f t="shared" si="98"/>
         <v>470966.16190909088</v>
       </c>
-      <c r="M372" s="169">
-        <f t="shared" si="95"/>
+      <c r="M372" s="164">
+        <f t="shared" si="98"/>
         <v>399525.55276136356</v>
       </c>
-      <c r="N372" s="169">
-        <f t="shared" si="91"/>
+      <c r="N372" s="164">
+        <f t="shared" si="94"/>
         <v>5852070.915504545</v>
       </c>
     </row>
@@ -10214,124 +10216,124 @@
         <v>1635123.3513727272</v>
       </c>
       <c r="C373" s="101">
-        <f t="shared" ref="C373:M373" si="96">SUM(C368:C372)</f>
+        <f t="shared" ref="C373:M373" si="99">SUM(C368:C372)</f>
         <v>1670200.6458000001</v>
       </c>
       <c r="D373" s="101">
-        <f t="shared" si="96"/>
+        <f t="shared" si="99"/>
         <v>1842678.0515636364</v>
       </c>
       <c r="E373" s="101">
-        <f t="shared" si="96"/>
+        <f t="shared" si="99"/>
         <v>1946334.2968818182</v>
       </c>
       <c r="F373" s="101">
-        <f t="shared" si="96"/>
+        <f t="shared" si="99"/>
         <v>2013621.158390909</v>
       </c>
       <c r="G373" s="101">
-        <f t="shared" si="96"/>
+        <f t="shared" si="99"/>
         <v>1943331.2263</v>
       </c>
       <c r="H373" s="101">
-        <f t="shared" si="96"/>
+        <f t="shared" si="99"/>
         <v>2155169.1973272725</v>
       </c>
       <c r="I373" s="101">
-        <f t="shared" si="96"/>
+        <f t="shared" si="99"/>
         <v>2422933.7340404545</v>
       </c>
       <c r="J373" s="101">
-        <f t="shared" si="96"/>
+        <f t="shared" si="99"/>
         <v>2194964.541855</v>
       </c>
       <c r="K373" s="101">
-        <f t="shared" si="96"/>
+        <f t="shared" si="99"/>
         <v>1998809.5663477276</v>
       </c>
       <c r="L373" s="101">
-        <f t="shared" si="96"/>
+        <f t="shared" si="99"/>
         <v>1758336.5564545454</v>
       </c>
       <c r="M373" s="101">
-        <f t="shared" si="96"/>
+        <f t="shared" si="99"/>
         <v>1640590.973443182</v>
       </c>
       <c r="N373" s="101">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>23222093.299777269</v>
       </c>
     </row>
     <row r="374" spans="1:14">
       <c r="A374" s="100"/>
-      <c r="B374" s="172"/>
-      <c r="C374" s="172"/>
-      <c r="D374" s="172"/>
-      <c r="E374" s="172"/>
-      <c r="F374" s="172"/>
-      <c r="G374" s="172"/>
-      <c r="H374" s="172"/>
-      <c r="I374" s="172"/>
-      <c r="J374" s="172"/>
-      <c r="K374" s="172"/>
-      <c r="L374" s="172"/>
-      <c r="M374" s="172"/>
-      <c r="N374" s="172"/>
+      <c r="B374" s="167"/>
+      <c r="C374" s="167"/>
+      <c r="D374" s="167"/>
+      <c r="E374" s="167"/>
+      <c r="F374" s="167"/>
+      <c r="G374" s="167"/>
+      <c r="H374" s="167"/>
+      <c r="I374" s="167"/>
+      <c r="J374" s="167"/>
+      <c r="K374" s="167"/>
+      <c r="L374" s="167"/>
+      <c r="M374" s="167"/>
+      <c r="N374" s="167"/>
     </row>
     <row r="375" spans="1:14">
       <c r="A375" s="98" t="s">
         <v>221</v>
       </c>
-      <c r="B375" s="170">
+      <c r="B375" s="165">
         <f>B366-B373</f>
         <v>634592.92175102234</v>
       </c>
-      <c r="C375" s="170">
+      <c r="C375" s="165">
         <f>C366-C373</f>
         <v>655073.40502499975</v>
       </c>
-      <c r="D375" s="170">
-        <f t="shared" ref="D375:M375" si="97">D366-D373</f>
+      <c r="D375" s="165">
+        <f t="shared" ref="D375:M375" si="100">D366-D373</f>
         <v>674190.61263636313</v>
       </c>
-      <c r="E375" s="170">
-        <f t="shared" si="97"/>
+      <c r="E375" s="165">
+        <f t="shared" si="100"/>
         <v>673033.74506818131</v>
       </c>
-      <c r="F375" s="170">
-        <f t="shared" si="97"/>
+      <c r="F375" s="165">
+        <f t="shared" si="100"/>
         <v>596455.96125909081</v>
       </c>
-      <c r="G375" s="170">
-        <f t="shared" si="97"/>
+      <c r="G375" s="165">
+        <f t="shared" si="100"/>
         <v>624227.90547500015</v>
       </c>
-      <c r="H375" s="170">
-        <f t="shared" si="97"/>
+      <c r="H375" s="165">
+        <f t="shared" si="100"/>
         <v>487769.53187272744</v>
       </c>
-      <c r="I375" s="170">
-        <f t="shared" si="97"/>
+      <c r="I375" s="165">
+        <f t="shared" si="100"/>
         <v>677967.99625954544</v>
       </c>
-      <c r="J375" s="170">
-        <f t="shared" si="97"/>
+      <c r="J375" s="165">
+        <f t="shared" si="100"/>
         <v>1174944.7082699998</v>
       </c>
-      <c r="K375" s="170">
-        <f t="shared" si="97"/>
+      <c r="K375" s="165">
+        <f t="shared" si="100"/>
         <v>1217230.4336272725</v>
       </c>
-      <c r="L375" s="170">
-        <f t="shared" si="97"/>
+      <c r="L375" s="165">
+        <f t="shared" si="100"/>
         <v>1069601.4085954544</v>
       </c>
-      <c r="M375" s="170">
-        <f t="shared" si="97"/>
+      <c r="M375" s="165">
+        <f t="shared" si="100"/>
         <v>826315.68250681763</v>
       </c>
-      <c r="N375" s="170">
-        <f t="shared" si="91"/>
+      <c r="N375" s="165">
+        <f t="shared" si="94"/>
         <v>9311404.3123464752</v>
       </c>
     </row>
@@ -10339,151 +10341,199 @@
       <c r="A376" s="98" t="s">
         <v>222</v>
       </c>
-      <c r="B376" s="171">
+      <c r="B376" s="166">
         <f>B375</f>
         <v>634592.92175102234</v>
       </c>
-      <c r="C376" s="171">
+      <c r="C376" s="166">
         <f>C375+B376</f>
         <v>1289666.3267760221</v>
       </c>
-      <c r="D376" s="171">
-        <f t="shared" ref="D376:M376" si="98">D375+C376</f>
+      <c r="D376" s="166">
+        <f t="shared" ref="D376:M376" si="101">D375+C376</f>
         <v>1963856.9394123852</v>
       </c>
-      <c r="E376" s="171">
-        <f t="shared" si="98"/>
+      <c r="E376" s="166">
+        <f t="shared" si="101"/>
         <v>2636890.6844805665</v>
       </c>
-      <c r="F376" s="171">
-        <f t="shared" si="98"/>
+      <c r="F376" s="166">
+        <f t="shared" si="101"/>
         <v>3233346.6457396573</v>
       </c>
-      <c r="G376" s="171">
-        <f t="shared" si="98"/>
+      <c r="G376" s="166">
+        <f t="shared" si="101"/>
         <v>3857574.5512146577</v>
       </c>
-      <c r="H376" s="171">
-        <f t="shared" si="98"/>
+      <c r="H376" s="166">
+        <f t="shared" si="101"/>
         <v>4345344.0830873847</v>
       </c>
-      <c r="I376" s="171">
-        <f t="shared" si="98"/>
+      <c r="I376" s="166">
+        <f t="shared" si="101"/>
         <v>5023312.0793469306</v>
       </c>
-      <c r="J376" s="171">
-        <f t="shared" si="98"/>
+      <c r="J376" s="166">
+        <f t="shared" si="101"/>
         <v>6198256.7876169309</v>
       </c>
-      <c r="K376" s="171">
-        <f t="shared" si="98"/>
+      <c r="K376" s="166">
+        <f t="shared" si="101"/>
         <v>7415487.2212442029</v>
       </c>
-      <c r="L376" s="171">
-        <f t="shared" si="98"/>
+      <c r="L376" s="166">
+        <f t="shared" si="101"/>
         <v>8485088.6298396569</v>
       </c>
-      <c r="M376" s="171">
-        <f t="shared" si="98"/>
+      <c r="M376" s="166">
+        <f t="shared" si="101"/>
         <v>9311404.3123464752</v>
       </c>
-      <c r="N376" s="171">
-        <f t="shared" si="91"/>
+      <c r="N376" s="166">
+        <f t="shared" si="94"/>
         <v>54394821.182855889</v>
       </c>
     </row>
-    <row r="378" spans="1:14" ht="18.75">
-      <c r="A378" s="26" t="s">
+    <row r="377" spans="1:14">
+      <c r="A377" s="176"/>
+      <c r="B377" s="177"/>
+      <c r="C377" s="177"/>
+      <c r="D377" s="177"/>
+      <c r="E377" s="177"/>
+      <c r="F377" s="177"/>
+      <c r="G377" s="177"/>
+      <c r="H377" s="177"/>
+      <c r="I377" s="177"/>
+      <c r="J377" s="177"/>
+      <c r="K377" s="177"/>
+      <c r="L377" s="177"/>
+      <c r="M377" s="177"/>
+      <c r="N377" s="177"/>
+    </row>
+    <row r="378" spans="1:14">
+      <c r="A378" s="176"/>
+      <c r="B378" s="177"/>
+      <c r="C378" s="177"/>
+      <c r="D378" s="177"/>
+      <c r="E378" s="177"/>
+      <c r="F378" s="177"/>
+      <c r="G378" s="177"/>
+      <c r="H378" s="177"/>
+      <c r="I378" s="177"/>
+      <c r="J378" s="177"/>
+      <c r="K378" s="177"/>
+      <c r="L378" s="177"/>
+      <c r="M378" s="177"/>
+      <c r="N378" s="177"/>
+    </row>
+    <row r="379" spans="1:14">
+      <c r="A379" s="176"/>
+      <c r="B379" s="177"/>
+      <c r="C379" s="177"/>
+      <c r="D379" s="177"/>
+      <c r="E379" s="177"/>
+      <c r="F379" s="177"/>
+      <c r="G379" s="177"/>
+      <c r="H379" s="177"/>
+      <c r="I379" s="177"/>
+      <c r="J379" s="177"/>
+      <c r="K379" s="177"/>
+      <c r="L379" s="177"/>
+      <c r="M379" s="177"/>
+      <c r="N379" s="177"/>
+    </row>
+    <row r="381" spans="1:14" ht="18.75">
+      <c r="A381" s="26" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="379" spans="1:14">
-      <c r="A379" s="99" t="s">
+    <row r="382" spans="1:14">
+      <c r="A382" s="99" t="s">
         <v>226</v>
       </c>
-      <c r="B379" s="99" t="s">
+      <c r="B382" s="99" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="380" spans="1:14">
-      <c r="A380" s="81" t="s">
+    <row r="383" spans="1:14">
+      <c r="A383" s="81" t="s">
         <v>174</v>
       </c>
-      <c r="B380" s="101">
+      <c r="B383" s="101">
         <v>32533497.612123746</v>
       </c>
     </row>
-    <row r="381" spans="1:14">
-      <c r="A381" s="98" t="s">
+    <row r="384" spans="1:14">
+      <c r="A384" s="98" t="s">
         <v>216</v>
       </c>
-      <c r="B381" s="97"/>
-    </row>
-    <row r="382" spans="1:14">
-      <c r="A382" s="132" t="s">
-        <v>217</v>
-      </c>
-      <c r="B382" s="169">
-        <v>5945408.9325000001</v>
-      </c>
-    </row>
-    <row r="383" spans="1:14">
-      <c r="A383" s="132" t="s">
-        <v>218</v>
-      </c>
-      <c r="B383" s="169">
-        <v>950000</v>
-      </c>
-    </row>
-    <row r="384" spans="1:14">
-      <c r="A384" s="132" t="s">
-        <v>128</v>
-      </c>
-      <c r="B384" s="169">
-        <v>8774316.9085000008</v>
-      </c>
+      <c r="B384" s="97"/>
     </row>
     <row r="385" spans="1:2">
       <c r="A385" s="132" t="s">
-        <v>167</v>
-      </c>
-      <c r="B385" s="169">
-        <v>1700296.5432727272</v>
+        <v>217</v>
+      </c>
+      <c r="B385" s="164">
+        <v>5945408.9325000001</v>
       </c>
     </row>
     <row r="386" spans="1:2">
       <c r="A386" s="132" t="s">
+        <v>218</v>
+      </c>
+      <c r="B386" s="164">
+        <v>950000</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2">
+      <c r="A387" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="B387" s="164">
+        <v>8774316.9085000008</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2">
+      <c r="A388" s="132" t="s">
+        <v>167</v>
+      </c>
+      <c r="B388" s="164">
+        <v>1700296.5432727272</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2">
+      <c r="A389" s="132" t="s">
         <v>175</v>
       </c>
-      <c r="B386" s="169">
+      <c r="B389" s="164">
         <v>5852070.915504545</v>
       </c>
     </row>
-    <row r="387" spans="1:2">
-      <c r="A387" s="100" t="s">
+    <row r="390" spans="1:2">
+      <c r="A390" s="100" t="s">
         <v>220</v>
       </c>
-      <c r="B387" s="101">
+      <c r="B390" s="101">
         <v>23222093.299777269</v>
       </c>
     </row>
-    <row r="388" spans="1:2">
-      <c r="A388" s="100"/>
-      <c r="B388" s="172"/>
-    </row>
-    <row r="389" spans="1:2">
-      <c r="A389" s="98" t="s">
+    <row r="391" spans="1:2">
+      <c r="A391" s="100"/>
+      <c r="B391" s="167"/>
+    </row>
+    <row r="392" spans="1:2">
+      <c r="A392" s="98" t="s">
         <v>221</v>
       </c>
-      <c r="B389" s="170">
+      <c r="B392" s="165">
         <v>9311404.3123464752</v>
       </c>
     </row>
-    <row r="390" spans="1:2">
-      <c r="A390" s="98" t="s">
+    <row r="393" spans="1:2">
+      <c r="A393" s="98" t="s">
         <v>222</v>
       </c>
-      <c r="B390" s="171">
+      <c r="B393" s="166">
         <v>54394821.182855889</v>
       </c>
     </row>
@@ -10495,7 +10545,7 @@
     <mergeCell ref="D320:E320"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="44" fitToHeight="16" orientation="landscape" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+  <pageSetup scale="43" fitToHeight="16" orientation="landscape" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="314" max="16383" man="1"/>
   </rowBreaks>

</xml_diff>